<commit_message>
Just for recording: on the way to implement of communication. * NoPageSample implemented * Persist loginInfo into LocalStorage * overlay display on communicating (not tested yet) * Stores to control communication and authentication are implemented. * TODO:   * Test local json file for debugging   * Communicate real server.
</commit_message>
<xml_diff>
--- a/meta/samples/pages/LoginSample.xlsx
+++ b/meta/samples/pages/LoginSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/samples/pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89B523F-7AD3-A344-BD81-7C743A023A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107AA104-4605-2C42-9CB5-3C7E881E0075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21600" yWindow="7800" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,11 +17,12 @@
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="adjustDefaultValue">config!$J$4:$J$5</definedName>
-    <definedName name="adjustFieldName">config!$H$4:$H$5</definedName>
-    <definedName name="adjustFiledName">config!$H$4:$H$5</definedName>
+    <definedName name="adjustDefaultValue">config!$L$4:$L$5</definedName>
+    <definedName name="adjustFieldName">config!$J$4:$J$5</definedName>
+    <definedName name="adjustFiledName">config!$J$4:$J$5</definedName>
     <definedName name="componentKind">config!$B$4:$B$5</definedName>
-    <definedName name="createToString">config!$F$4:$F$5</definedName>
+    <definedName name="createToString">config!$H$4:$H$5</definedName>
+    <definedName name="httpMethod">config!$F$4:$F$8</definedName>
     <definedName name="yesNo">config!$D$4:$D$5</definedName>
     <definedName name="チェック種別" localSheetId="1">#REF!</definedName>
     <definedName name="チェック種別">#REF!</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
   <si>
     <t>パッケージ</t>
   </si>
@@ -584,13 +585,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>クラス名</t>
-    <rPh sb="3" eb="4">
-      <t xml:space="preserve">メイ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
       <t xml:space="preserve">セツメイ </t>
@@ -871,6 +865,44 @@
     <rPh sb="7" eb="9">
       <t xml:space="preserve">ガメｎ </t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>メソッド</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>HTTPメソッド</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>認証APIです。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ニンショウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { LoginSamplePostRequest } from "%/samples/api/LoginSamplePostRequest"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -878,7 +910,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -923,6 +955,12 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -962,7 +1000,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1512,12 +1550,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1671,9 +1754,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1682,6 +1762,45 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1691,45 +1810,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2143,8 +2241,8 @@
   </sheetPr>
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2162,7 +2260,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="19">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>50</v>
@@ -2180,7 +2278,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2196,7 +2294,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -2213,12 +2311,12 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
       <c r="F7" s="34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
@@ -2230,7 +2328,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
@@ -2247,7 +2345,7 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="11"/>
@@ -2259,12 +2357,12 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="102"/>
+      <c r="B10" s="100"/>
       <c r="C10" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
@@ -2276,12 +2374,12 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="102"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
@@ -2293,10 +2391,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="102"/>
+      <c r="B12" s="100"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2310,10 +2408,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="86" t="s">
         <v>48</v>
       </c>
@@ -2331,11 +2429,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="103" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="104"/>
-      <c r="E14" s="105"/>
+      <c r="C14" s="101" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2349,7 +2447,7 @@
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="8"/>
@@ -2443,14 +2541,14 @@
     </row>
     <row r="21" spans="1:13" s="32" customFormat="1">
       <c r="A21" s="62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="63"/>
       <c r="C21" s="64" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21"/>
       <c r="F21"/>
@@ -2476,10 +2574,10 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="106" t="s">
+      <c r="A23" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="107"/>
+      <c r="B23" s="92"/>
       <c r="C23" s="64"/>
       <c r="D23" t="s">
         <v>58</v>
@@ -2506,10 +2604,10 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="106" t="s">
+      <c r="A25" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="107"/>
+      <c r="B25" s="92"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
@@ -2523,10 +2621,10 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="106" t="s">
+      <c r="A26" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="107"/>
+      <c r="B26" s="92"/>
       <c r="C26" s="64" t="s">
         <v>14</v>
       </c>
@@ -2552,7 +2650,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -2593,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
@@ -2692,7 +2790,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
@@ -2711,7 +2809,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" s="40"/>
       <c r="D37" s="40"/>
@@ -2730,7 +2828,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="49"/>
       <c r="D38" s="49"/>
@@ -2776,7 +2874,7 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="31"/>
       <c r="C41" s="31"/>
@@ -2813,8 +2911,12 @@
       <c r="M42" s="35"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="51"/>
-      <c r="B43" s="46"/>
+      <c r="A43" s="51">
+        <v>1</v>
+      </c>
+      <c r="B43" s="46" t="s">
+        <v>103</v>
+      </c>
       <c r="C43" s="38"/>
       <c r="D43" s="38"/>
       <c r="E43" s="39"/>
@@ -2878,7 +2980,7 @@
       <c r="D47" s="31"/>
       <c r="E47" s="81"/>
       <c r="F47" s="44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
@@ -2896,10 +2998,10 @@
         <v>63</v>
       </c>
       <c r="C48" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="42" t="s">
         <v>64</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>65</v>
       </c>
       <c r="E48" s="82"/>
       <c r="F48" s="67"/>
@@ -2912,10 +3014,18 @@
       <c r="M48" s="35"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="51"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="38"/>
+      <c r="A49" s="51">
+        <v>1</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="111" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="114" t="s">
+        <v>102</v>
+      </c>
       <c r="E49" s="39"/>
       <c r="F49" s="68"/>
       <c r="G49" s="68"/>
@@ -2929,8 +3039,8 @@
     <row r="50" spans="1:13">
       <c r="A50" s="51"/>
       <c r="B50" s="46"/>
-      <c r="C50" s="88"/>
-      <c r="D50" s="40"/>
+      <c r="C50" s="112"/>
+      <c r="D50" s="115"/>
       <c r="E50" s="41"/>
       <c r="F50" s="68"/>
       <c r="G50" s="68"/>
@@ -2944,8 +3054,8 @@
     <row r="51" spans="1:13">
       <c r="A51" s="52"/>
       <c r="B51" s="48"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="49"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="116"/>
       <c r="E51" s="50"/>
       <c r="F51" s="68"/>
       <c r="G51" s="68"/>
@@ -2973,7 +3083,7 @@
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
@@ -3001,7 +3111,7 @@
       <c r="D54" s="42"/>
       <c r="E54" s="82"/>
       <c r="F54" s="67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G54" s="67"/>
       <c r="H54" s="67"/>
@@ -3084,7 +3194,7 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="14"/>
@@ -3100,49 +3210,49 @@
       <c r="M60" s="15"/>
     </row>
     <row r="61" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A61" s="100" t="s">
+      <c r="A61" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="100" t="s">
+      <c r="B61" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="97" t="s">
+      <c r="C61" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="97" t="s">
+      <c r="D61" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="97" t="s">
+      <c r="E61" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F61" s="98" t="s">
+      <c r="F61" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="G61" s="98" t="s">
+      <c r="G61" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="H61" s="108" t="s">
-        <v>81</v>
-      </c>
-      <c r="I61" s="97" t="s">
+      <c r="H61" s="95" t="s">
+        <v>80</v>
+      </c>
+      <c r="I61" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="J61" s="97"/>
+      <c r="J61" s="93"/>
       <c r="K61" s="16"/>
       <c r="L61" s="17"/>
       <c r="M61" s="9"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="100"/>
-      <c r="B62" s="100"/>
-      <c r="C62" s="97"/>
-      <c r="D62" s="97"/>
-      <c r="E62" s="97"/>
-      <c r="F62" s="99"/>
-      <c r="G62" s="99"/>
-      <c r="H62" s="109"/>
-      <c r="I62" s="97"/>
-      <c r="J62" s="97"/>
+      <c r="A62" s="94"/>
+      <c r="B62" s="94"/>
+      <c r="C62" s="93"/>
+      <c r="D62" s="93"/>
+      <c r="E62" s="93"/>
+      <c r="F62" s="98"/>
+      <c r="G62" s="98"/>
+      <c r="H62" s="96"/>
+      <c r="I62" s="93"/>
+      <c r="J62" s="93"/>
       <c r="K62" s="18"/>
       <c r="L62" s="29"/>
       <c r="M62" s="15"/>
@@ -3469,7 +3579,7 @@
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B82" s="31"/>
       <c r="C82" s="31"/>
@@ -3565,7 +3675,7 @@
     <row r="88" spans="1:13">
       <c r="A88" s="13"/>
       <c r="B88" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C88" s="13"/>
       <c r="D88" s="13"/>
@@ -3578,7 +3688,7 @@
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
@@ -3594,41 +3704,41 @@
       <c r="M89" s="15"/>
     </row>
     <row r="90" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A90" s="100" t="s">
+      <c r="A90" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="100" t="s">
-        <v>68</v>
-      </c>
-      <c r="C90" s="97" t="s">
+      <c r="B90" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="C90" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="D90" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="D90" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="E90" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="F90" s="94"/>
-      <c r="G90" s="94"/>
-      <c r="H90" s="94"/>
-      <c r="I90" s="96"/>
-      <c r="J90" s="97"/>
+      <c r="E90" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="F90" s="104"/>
+      <c r="G90" s="104"/>
+      <c r="H90" s="104"/>
+      <c r="I90" s="106"/>
+      <c r="J90" s="93"/>
       <c r="K90" s="16"/>
       <c r="L90" s="17"/>
       <c r="M90" s="9"/>
     </row>
     <row r="91" spans="1:13">
-      <c r="A91" s="100"/>
-      <c r="B91" s="100"/>
-      <c r="C91" s="97"/>
-      <c r="D91" s="97"/>
-      <c r="E91" s="97"/>
-      <c r="F91" s="95"/>
-      <c r="G91" s="95"/>
-      <c r="H91" s="95"/>
-      <c r="I91" s="96"/>
-      <c r="J91" s="97"/>
+      <c r="A91" s="94"/>
+      <c r="B91" s="94"/>
+      <c r="C91" s="93"/>
+      <c r="D91" s="93"/>
+      <c r="E91" s="93"/>
+      <c r="F91" s="105"/>
+      <c r="G91" s="105"/>
+      <c r="H91" s="105"/>
+      <c r="I91" s="106"/>
+      <c r="J91" s="93"/>
       <c r="K91" s="18"/>
       <c r="L91" s="29"/>
       <c r="M91" s="15"/>
@@ -3641,10 +3751,10 @@
       <c r="C92" s="78"/>
       <c r="D92" s="20"/>
       <c r="E92" s="20"/>
-      <c r="F92" s="90"/>
-      <c r="G92" s="92"/>
-      <c r="H92" s="92"/>
-      <c r="I92" s="90"/>
+      <c r="F92" s="87"/>
+      <c r="G92" s="89"/>
+      <c r="H92" s="89"/>
+      <c r="I92" s="87"/>
       <c r="J92" s="21"/>
       <c r="K92" s="21"/>
       <c r="L92" s="28"/>
@@ -3659,10 +3769,10 @@
       <c r="C93" s="78"/>
       <c r="D93" s="20"/>
       <c r="E93" s="20"/>
-      <c r="F93" s="90"/>
-      <c r="G93" s="92"/>
-      <c r="H93" s="92"/>
-      <c r="I93" s="90"/>
+      <c r="F93" s="87"/>
+      <c r="G93" s="89"/>
+      <c r="H93" s="89"/>
+      <c r="I93" s="87"/>
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
       <c r="L93" s="28"/>
@@ -3677,10 +3787,10 @@
       <c r="C94" s="79"/>
       <c r="D94" s="20"/>
       <c r="E94" s="20"/>
-      <c r="F94" s="90"/>
-      <c r="G94" s="92"/>
-      <c r="H94" s="92"/>
-      <c r="I94" s="90"/>
+      <c r="F94" s="87"/>
+      <c r="G94" s="89"/>
+      <c r="H94" s="89"/>
+      <c r="I94" s="87"/>
       <c r="J94" s="21"/>
       <c r="K94" s="21"/>
       <c r="L94" s="22"/>
@@ -3695,10 +3805,10 @@
       <c r="C95" s="80"/>
       <c r="D95" s="20"/>
       <c r="E95" s="20"/>
-      <c r="F95" s="90"/>
-      <c r="G95" s="92"/>
-      <c r="H95" s="92"/>
-      <c r="I95" s="90"/>
+      <c r="F95" s="87"/>
+      <c r="G95" s="89"/>
+      <c r="H95" s="89"/>
+      <c r="I95" s="87"/>
       <c r="J95" s="21"/>
       <c r="K95" s="21"/>
       <c r="L95" s="22"/>
@@ -3713,10 +3823,10 @@
       <c r="C96" s="80"/>
       <c r="D96" s="20"/>
       <c r="E96" s="20"/>
-      <c r="F96" s="90"/>
-      <c r="G96" s="92"/>
-      <c r="H96" s="92"/>
-      <c r="I96" s="90"/>
+      <c r="F96" s="87"/>
+      <c r="G96" s="89"/>
+      <c r="H96" s="89"/>
+      <c r="I96" s="87"/>
       <c r="J96" s="21"/>
       <c r="K96" s="21"/>
       <c r="L96" s="22"/>
@@ -3731,10 +3841,10 @@
       <c r="C97" s="80"/>
       <c r="D97" s="74"/>
       <c r="E97" s="74"/>
-      <c r="F97" s="91"/>
-      <c r="G97" s="93"/>
-      <c r="H97" s="93"/>
-      <c r="I97" s="91"/>
+      <c r="F97" s="88"/>
+      <c r="G97" s="90"/>
+      <c r="H97" s="90"/>
+      <c r="I97" s="88"/>
       <c r="J97" s="76"/>
       <c r="K97" s="76"/>
       <c r="L97" s="77"/>
@@ -3749,10 +3859,10 @@
       <c r="C98" s="80"/>
       <c r="D98" s="20"/>
       <c r="E98" s="20"/>
-      <c r="F98" s="90"/>
-      <c r="G98" s="92"/>
-      <c r="H98" s="92"/>
-      <c r="I98" s="90"/>
+      <c r="F98" s="87"/>
+      <c r="G98" s="89"/>
+      <c r="H98" s="89"/>
+      <c r="I98" s="87"/>
       <c r="J98" s="21"/>
       <c r="K98" s="21"/>
       <c r="L98" s="22"/>
@@ -3760,6 +3870,21 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="H90:H91"/>
+    <mergeCell ref="I90:J91"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="I61:J62"/>
@@ -3771,24 +3896,9 @@
     <mergeCell ref="H61:H62"/>
     <mergeCell ref="F61:F62"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="H90:H91"/>
-    <mergeCell ref="I90:J91"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="G90:G91"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E102:H102" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
@@ -3805,6 +3915,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49:C51" xr:uid="{7DF12094-1903-BC49-BDF2-8CDB3E7A15D0}">
+      <formula1>httpMethod</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
   <pageSetup paperSize="9" scale="82" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -3819,10 +3932,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F4" sqref="F4:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -3832,14 +3945,16 @@
     <col min="5" max="5" width="8.83203125" style="55" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="55" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="55" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="55" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="55" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="251" width="8.83203125" style="55" customWidth="1"/>
-    <col min="252" max="16384" width="10.83203125" style="55"/>
+    <col min="11" max="11" width="8.83203125" style="55" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
+    <col min="13" max="253" width="8.83203125" style="55" customWidth="1"/>
+    <col min="254" max="16384" width="10.83203125" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19">
+    <row r="1" spans="1:12" ht="19">
       <c r="A1" s="53" t="s">
         <v>8</v>
       </c>
@@ -3851,11 +3966,13 @@
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="B3" s="56" t="s">
         <v>25</v>
       </c>
@@ -3863,33 +3980,37 @@
         <v>31</v>
       </c>
       <c r="F3" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="J3" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="L3" s="56" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="B4" s="57" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="107"/>
       <c r="H4" s="58"/>
       <c r="J4" s="58"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" s="58"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="B5" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="60"/>
-      <c r="F5" s="60" t="s">
-        <v>13</v>
+      <c r="F5" s="108" t="s">
+        <v>97</v>
       </c>
       <c r="H5" s="60" t="s">
         <v>13</v>
@@ -3897,9 +4018,25 @@
       <c r="J5" s="60" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" s="60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="B6" s="61"/>
+      <c r="F6" s="108" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="F7" s="109" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="F8" s="110" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6"/>

</xml_diff>

<commit_message>
* implement force reload option with befreRouteLeave. * on the way of implement login and sessionToken.
</commit_message>
<xml_diff>
--- a/meta/samples/pages/LoginSample.xlsx
+++ b/meta/samples/pages/LoginSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/samples/pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107AA104-4605-2C42-9CB5-3C7E881E0075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B506771-5CB3-8E41-8559-FD434B10CAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="7800" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="108">
   <si>
     <t>パッケージ</t>
   </si>
@@ -818,10 +818,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>import {ErrorMessage, Field, Form} from "vee-validate"</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Field</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -903,6 +899,56 @@
   </si>
   <si>
     <t>import { LoginSamplePostRequest } from "%/samples/api/LoginSamplePostRequest"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { RouterHooks } from "@/utils/RouterHooks"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { ErrorMessage, Field, Form } from "vee-validate"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>BeforeRouteLeave関数名</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>RouterHooks.beforeRouteLeave</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* BeforeRouteLeave関数を実装する場合はここに関数名を定義し、Vueコンポーネント定義・ヘッダ情報（コンポーネント定義用）に関数のインポートを定義します。 */</t>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t xml:space="preserve">カンスウメイヲ </t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t xml:space="preserve">テイギシ </t>
+    </rPh>
+    <rPh sb="47" eb="50">
+      <t xml:space="preserve">テイギヨウ </t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="80" eb="82">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1600,7 +1646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1762,54 +1808,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1828,6 +1826,57 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2239,10 +2288,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2294,7 +2343,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
@@ -2311,7 +2360,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
@@ -2328,7 +2377,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
@@ -2345,7 +2394,7 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="11"/>
@@ -2357,12 +2406,12 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="100"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
@@ -2374,12 +2423,12 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="100"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
@@ -2391,10 +2440,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2408,10 +2457,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="86" t="s">
         <v>48</v>
       </c>
@@ -2429,11 +2478,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="101" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="102"/>
-      <c r="E14" s="103"/>
+      <c r="C14" s="110" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="111"/>
+      <c r="E14" s="112"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2574,10 +2623,10 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="91" t="s">
+      <c r="A23" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="92"/>
+      <c r="B23" s="114"/>
       <c r="C23" s="64"/>
       <c r="D23" t="s">
         <v>58</v>
@@ -2589,31 +2638,31 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="63"/>
+      <c r="A24" s="113" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="114"/>
       <c r="C24" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24"/>
+        <v>106</v>
+      </c>
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
+      <c r="G24"/>
+      <c r="H24"/>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="91" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="92"/>
+      <c r="A25" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="63"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
+      <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" s="66"/>
@@ -2621,96 +2670,98 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="91" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="92"/>
+      <c r="A26" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="114"/>
       <c r="C26" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D26"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" s="66"/>
       <c r="H26" s="66"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:13" s="37" customFormat="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="30" t="s">
+    <row r="27" spans="1:13" s="32" customFormat="1">
+      <c r="A27" s="113" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="114"/>
+      <c r="C27" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:13" s="37" customFormat="1">
+      <c r="A28" s="34"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="44" t="s">
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="47" t="s">
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B30" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="35"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="51">
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="35"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="51">
         <v>1</v>
       </c>
-      <c r="B30" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="51"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
+      <c r="B31" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="68"/>
       <c r="G31" s="68"/>
       <c r="H31" s="68"/>
@@ -2720,119 +2771,113 @@
       <c r="L31" s="36"/>
       <c r="M31" s="35"/>
     </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="52"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="35"/>
+    <row r="32" spans="1:13" s="32" customFormat="1">
+      <c r="A32" s="51">
+        <v>2</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="117"/>
+      <c r="D32" s="117"/>
+      <c r="E32" s="118"/>
+      <c r="F32" s="119"/>
+      <c r="G32" s="119"/>
+      <c r="H32" s="119"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
+      <c r="A33" s="51"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="35"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="52"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="35"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="44" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="47" t="s">
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B37" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="51">
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="35"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="51">
         <v>1</v>
       </c>
-      <c r="B36" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="51">
-        <v>2</v>
-      </c>
-      <c r="B37" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="35"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="52">
-        <v>3</v>
-      </c>
-      <c r="B38" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50"/>
+      <c r="B38" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="68"/>
       <c r="G38" s="68"/>
       <c r="H38" s="68"/>
@@ -2843,11 +2888,15 @@
       <c r="M38" s="35"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="83"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
+      <c r="A39" s="51">
+        <v>2</v>
+      </c>
+      <c r="B39" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
       <c r="F39" s="68"/>
       <c r="G39" s="68"/>
       <c r="H39" s="68"/>
@@ -2858,11 +2907,15 @@
       <c r="M39" s="35"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="83"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="68"/>
+      <c r="A40" s="52">
+        <v>3</v>
+      </c>
+      <c r="B40" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="50"/>
       <c r="F40" s="68"/>
       <c r="G40" s="68"/>
       <c r="H40" s="68"/>
@@ -2873,83 +2926,83 @@
       <c r="M40" s="35"/>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="83"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="35"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="83"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="36"/>
+      <c r="M42" s="35"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="44" t="s">
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="47" t="s">
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+      <c r="M43" s="43"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B44" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="67"/>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="51">
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="45"/>
+      <c r="L44" s="45"/>
+      <c r="M44" s="35"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="51">
         <v>1</v>
       </c>
-      <c r="B43" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="35"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="51"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="35"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="52"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="50"/>
+      <c r="B45" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="39"/>
       <c r="F45" s="68"/>
       <c r="G45" s="68"/>
       <c r="H45" s="68"/>
@@ -2960,103 +3013,103 @@
       <c r="M45" s="35"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
+      <c r="A46" s="51"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="35"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="52"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="35"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="44" t="s">
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="47" t="s">
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B50" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="42" t="s">
+      <c r="C50" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="82"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="67"/>
-      <c r="I48" s="67"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
-      <c r="M48" s="35"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="51">
+      <c r="E50" s="82"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="67"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="35"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="51">
         <v>1</v>
       </c>
-      <c r="B49" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" s="111" t="s">
+      <c r="B51" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="D49" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
-      <c r="M49" s="35"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="51"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="112"/>
-      <c r="D50" s="115"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="36"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="35"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="52"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="113"/>
-      <c r="D51" s="116"/>
-      <c r="E51" s="50"/>
+      <c r="E51" s="39"/>
       <c r="F51" s="68"/>
       <c r="G51" s="68"/>
       <c r="H51" s="68"/>
@@ -3067,11 +3120,11 @@
       <c r="M51" s="35"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="83"/>
-      <c r="B52" s="84"/>
-      <c r="C52" s="85"/>
-      <c r="D52" s="85"/>
-      <c r="E52" s="85"/>
+      <c r="A52" s="51"/>
+      <c r="B52" s="46"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="99"/>
+      <c r="E52" s="41"/>
       <c r="F52" s="68"/>
       <c r="G52" s="68"/>
       <c r="H52" s="68"/>
@@ -3082,81 +3135,81 @@
       <c r="M52" s="35"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="52"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="100"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="68"/>
+      <c r="H53" s="68"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="35"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="83"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="85"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="68"/>
+      <c r="H54" s="68"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="36"/>
+      <c r="M54" s="35"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="81"/>
-      <c r="F53" s="44" t="s">
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-      <c r="M53" s="43"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="47" t="s">
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="43"/>
+      <c r="M55" s="43"/>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B56" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="82"/>
-      <c r="F54" s="67" t="s">
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="82"/>
+      <c r="F56" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="G54" s="67"/>
-      <c r="H54" s="67"/>
-      <c r="I54" s="67"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="45"/>
-      <c r="L54" s="45"/>
-      <c r="M54" s="35"/>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="51"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="35"/>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="51"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="68"/>
-      <c r="G56" s="68"/>
-      <c r="H56" s="68"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
-      <c r="L56" s="36"/>
+      <c r="G56" s="67"/>
+      <c r="H56" s="67"/>
+      <c r="I56" s="67"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="45"/>
+      <c r="L56" s="45"/>
       <c r="M56" s="35"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="52"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="50"/>
+      <c r="A57" s="51"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="39"/>
       <c r="F57" s="68"/>
       <c r="G57" s="68"/>
       <c r="H57" s="68"/>
@@ -3167,138 +3220,132 @@
       <c r="M57" s="35"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
+      <c r="A58" s="51"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="68"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="36"/>
+      <c r="K58" s="36"/>
+      <c r="L58" s="36"/>
+      <c r="M58" s="35"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13" t="s">
+      <c r="A59" s="52"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="68"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="36"/>
+      <c r="K59" s="36"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="35"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="13"/>
+      <c r="B61" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="3" t="s">
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="6"/>
-      <c r="M60" s="15"/>
-    </row>
-    <row r="61" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A61" s="94" t="s">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="15"/>
+    </row>
+    <row r="63" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A63" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="94" t="s">
+      <c r="B63" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="93" t="s">
+      <c r="C63" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="93" t="s">
+      <c r="D63" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="93" t="s">
+      <c r="E63" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="F61" s="97" t="s">
+      <c r="F63" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="G61" s="97" t="s">
+      <c r="G63" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="H61" s="95" t="s">
+      <c r="H63" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="I61" s="93" t="s">
+      <c r="I63" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="J61" s="93"/>
-      <c r="K61" s="16"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="9"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="94"/>
-      <c r="B62" s="94"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="93"/>
-      <c r="E62" s="93"/>
-      <c r="F62" s="98"/>
-      <c r="G62" s="98"/>
-      <c r="H62" s="96"/>
-      <c r="I62" s="93"/>
-      <c r="J62" s="93"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="29"/>
-      <c r="M62" s="15"/>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" s="19">
-        <v>1</v>
-      </c>
-      <c r="B63" s="71"/>
-      <c r="C63" s="78"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="69"/>
-      <c r="H63" s="69"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="28"/>
-      <c r="M63" s="15"/>
+      <c r="J63" s="104"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="9"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="19">
-        <f>A63+1</f>
-        <v>2</v>
-      </c>
-      <c r="B64" s="71"/>
-      <c r="C64" s="78"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="69"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="21"/>
-      <c r="K64" s="21"/>
-      <c r="L64" s="28"/>
+      <c r="A64" s="107"/>
+      <c r="B64" s="107"/>
+      <c r="C64" s="104"/>
+      <c r="D64" s="104"/>
+      <c r="E64" s="104"/>
+      <c r="F64" s="106"/>
+      <c r="G64" s="106"/>
+      <c r="H64" s="116"/>
+      <c r="I64" s="104"/>
+      <c r="J64" s="104"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="29"/>
       <c r="M64" s="15"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="19">
-        <f t="shared" ref="A65:A79" si="0">A64+1</f>
-        <v>3</v>
-      </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="79"/>
+        <v>1</v>
+      </c>
+      <c r="B65" s="71"/>
+      <c r="C65" s="78"/>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
@@ -3307,16 +3354,16 @@
       <c r="I65" s="20"/>
       <c r="J65" s="21"/>
       <c r="K65" s="21"/>
-      <c r="L65" s="22"/>
+      <c r="L65" s="28"/>
       <c r="M65" s="15"/>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B66" s="73"/>
-      <c r="C66" s="80"/>
+        <f>A65+1</f>
+        <v>2</v>
+      </c>
+      <c r="B66" s="71"/>
+      <c r="C66" s="78"/>
       <c r="D66" s="20"/>
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
@@ -3325,16 +3372,16 @@
       <c r="I66" s="20"/>
       <c r="J66" s="21"/>
       <c r="K66" s="21"/>
-      <c r="L66" s="22"/>
+      <c r="L66" s="28"/>
       <c r="M66" s="15"/>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="19">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B67" s="73"/>
-      <c r="C67" s="80"/>
+        <f t="shared" ref="A67:A81" si="0">A66+1</f>
+        <v>3</v>
+      </c>
+      <c r="B67" s="72"/>
+      <c r="C67" s="79"/>
       <c r="D67" s="20"/>
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
@@ -3349,25 +3396,25 @@
     <row r="68" spans="1:13">
       <c r="A68" s="19">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B68" s="73"/>
       <c r="C68" s="80"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="74"/>
-      <c r="J68" s="76"/>
-      <c r="K68" s="76"/>
-      <c r="L68" s="77"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="69"/>
+      <c r="H68" s="69"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="22"/>
       <c r="M68" s="15"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="19">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B69" s="73"/>
       <c r="C69" s="80"/>
@@ -3385,7 +3432,7 @@
     <row r="70" spans="1:13">
       <c r="A70" s="19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B70" s="73"/>
       <c r="C70" s="80"/>
@@ -3403,43 +3450,43 @@
     <row r="71" spans="1:13">
       <c r="A71" s="19">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B71" s="73"/>
       <c r="C71" s="80"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="74"/>
-      <c r="F71" s="74"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
-      <c r="I71" s="74"/>
-      <c r="J71" s="76"/>
-      <c r="K71" s="76"/>
-      <c r="L71" s="77"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="69"/>
+      <c r="H71" s="69"/>
+      <c r="I71" s="20"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="22"/>
       <c r="M71" s="15"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B72" s="73"/>
       <c r="C72" s="80"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="69"/>
-      <c r="H72" s="69"/>
-      <c r="I72" s="20"/>
-      <c r="J72" s="21"/>
-      <c r="K72" s="21"/>
-      <c r="L72" s="22"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="74"/>
+      <c r="G72" s="75"/>
+      <c r="H72" s="75"/>
+      <c r="I72" s="74"/>
+      <c r="J72" s="76"/>
+      <c r="K72" s="76"/>
+      <c r="L72" s="77"/>
       <c r="M72" s="15"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B73" s="73"/>
       <c r="C73" s="80"/>
@@ -3457,43 +3504,43 @@
     <row r="74" spans="1:13">
       <c r="A74" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B74" s="73"/>
       <c r="C74" s="80"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="76"/>
-      <c r="K74" s="76"/>
-      <c r="L74" s="77"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="69"/>
+      <c r="H74" s="69"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="22"/>
       <c r="M74" s="15"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B75" s="73"/>
       <c r="C75" s="80"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="69"/>
-      <c r="I75" s="20"/>
-      <c r="J75" s="21"/>
-      <c r="K75" s="21"/>
-      <c r="L75" s="22"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="74"/>
+      <c r="G75" s="75"/>
+      <c r="H75" s="75"/>
+      <c r="I75" s="74"/>
+      <c r="J75" s="76"/>
+      <c r="K75" s="76"/>
+      <c r="L75" s="77"/>
       <c r="M75" s="15"/>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="19">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B76" s="73"/>
       <c r="C76" s="80"/>
@@ -3511,43 +3558,43 @@
     <row r="77" spans="1:13">
       <c r="A77" s="19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B77" s="73"/>
       <c r="C77" s="80"/>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-      <c r="F77" s="74"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="74"/>
-      <c r="J77" s="76"/>
-      <c r="K77" s="76"/>
-      <c r="L77" s="77"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="69"/>
+      <c r="H77" s="69"/>
+      <c r="I77" s="20"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="22"/>
       <c r="M77" s="15"/>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="19">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B78" s="73"/>
       <c r="C78" s="80"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="69"/>
-      <c r="H78" s="69"/>
-      <c r="I78" s="20"/>
-      <c r="J78" s="21"/>
-      <c r="K78" s="21"/>
-      <c r="L78" s="22"/>
+      <c r="D78" s="74"/>
+      <c r="E78" s="74"/>
+      <c r="F78" s="74"/>
+      <c r="G78" s="75"/>
+      <c r="H78" s="75"/>
+      <c r="I78" s="74"/>
+      <c r="J78" s="76"/>
+      <c r="K78" s="76"/>
+      <c r="L78" s="77"/>
       <c r="M78" s="15"/>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B79" s="73"/>
       <c r="C79" s="80"/>
@@ -3563,94 +3610,100 @@
       <c r="M79" s="15"/>
     </row>
     <row r="80" spans="1:13">
-      <c r="A80" s="23"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="70"/>
-      <c r="H80" s="70"/>
-      <c r="I80" s="25"/>
-      <c r="J80" s="26"/>
-      <c r="K80" s="26"/>
-      <c r="L80" s="27"/>
+      <c r="A80" s="19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B80" s="73"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="69"/>
+      <c r="H80" s="69"/>
+      <c r="I80" s="20"/>
+      <c r="J80" s="21"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="22"/>
       <c r="M80" s="15"/>
     </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B81" s="73"/>
+      <c r="C81" s="80"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+      <c r="F81" s="74"/>
+      <c r="G81" s="75"/>
+      <c r="H81" s="75"/>
+      <c r="I81" s="74"/>
+      <c r="J81" s="76"/>
+      <c r="K81" s="76"/>
+      <c r="L81" s="77"/>
+      <c r="M81" s="15"/>
+    </row>
     <row r="82" spans="1:13">
-      <c r="A82" s="30" t="s">
+      <c r="A82" s="23"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="70"/>
+      <c r="H82" s="70"/>
+      <c r="I82" s="25"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="26"/>
+      <c r="L82" s="27"/>
+      <c r="M82" s="15"/>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B82" s="31"/>
-      <c r="C82" s="31"/>
-      <c r="D82" s="31"/>
-      <c r="E82" s="81"/>
-      <c r="F82" s="44" t="s">
+      <c r="B84" s="31"/>
+      <c r="C84" s="31"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="81"/>
+      <c r="F84" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G82" s="44"/>
-      <c r="H82" s="44"/>
-      <c r="I82" s="44"/>
-      <c r="J82" s="43"/>
-      <c r="K82" s="43"/>
-      <c r="L82" s="43"/>
-      <c r="M82" s="43"/>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="47" t="s">
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="44"/>
+      <c r="J84" s="43"/>
+      <c r="K84" s="43"/>
+      <c r="L84" s="43"/>
+      <c r="M84" s="43"/>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="42" t="s">
+      <c r="B85" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C83" s="42"/>
-      <c r="D83" s="42"/>
-      <c r="E83" s="82"/>
-      <c r="F83" s="67"/>
-      <c r="G83" s="67"/>
-      <c r="H83" s="67"/>
-      <c r="I83" s="67"/>
-      <c r="J83" s="44"/>
-      <c r="K83" s="45"/>
-      <c r="L83" s="45"/>
-      <c r="M83" s="35"/>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="51"/>
-      <c r="B84" s="46"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="36"/>
-      <c r="K84" s="36"/>
-      <c r="L84" s="36"/>
-      <c r="M84" s="35"/>
-    </row>
-    <row r="85" spans="1:13">
-      <c r="A85" s="51"/>
-      <c r="B85" s="46"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="41"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
-      <c r="I85" s="34"/>
-      <c r="J85" s="36"/>
-      <c r="K85" s="36"/>
-      <c r="L85" s="36"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="82"/>
+      <c r="F85" s="67"/>
+      <c r="G85" s="67"/>
+      <c r="H85" s="67"/>
+      <c r="I85" s="67"/>
+      <c r="J85" s="44"/>
+      <c r="K85" s="45"/>
+      <c r="L85" s="45"/>
       <c r="M85" s="35"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="52"/>
-      <c r="B86" s="48"/>
-      <c r="C86" s="49"/>
-      <c r="D86" s="49"/>
-      <c r="E86" s="50"/>
+      <c r="A86" s="51"/>
+      <c r="B86" s="46"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="39"/>
       <c r="F86" s="68"/>
       <c r="G86" s="68"/>
       <c r="H86" s="68"/>
@@ -3661,130 +3714,124 @@
       <c r="M86" s="35"/>
     </row>
     <row r="87" spans="1:13">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
+      <c r="A87" s="51"/>
+      <c r="B87" s="46"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="41"/>
+      <c r="F87" s="68"/>
+      <c r="G87" s="68"/>
+      <c r="H87" s="68"/>
+      <c r="I87" s="34"/>
+      <c r="J87" s="36"/>
+      <c r="K87" s="36"/>
+      <c r="L87" s="36"/>
+      <c r="M87" s="35"/>
     </row>
     <row r="88" spans="1:13">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13" t="s">
+      <c r="A88" s="52"/>
+      <c r="B88" s="48"/>
+      <c r="C88" s="49"/>
+      <c r="D88" s="49"/>
+      <c r="E88" s="50"/>
+      <c r="F88" s="68"/>
+      <c r="G88" s="68"/>
+      <c r="H88" s="68"/>
+      <c r="I88" s="34"/>
+      <c r="J88" s="36"/>
+      <c r="K88" s="36"/>
+      <c r="L88" s="36"/>
+      <c r="M88" s="35"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="13"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="13"/>
+      <c r="B90" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="3" t="s">
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="13"/>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="6"/>
-      <c r="M89" s="15"/>
-    </row>
-    <row r="90" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A90" s="94" t="s">
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="15"/>
+    </row>
+    <row r="92" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A92" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="94" t="s">
+      <c r="B92" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="C90" s="93" t="s">
+      <c r="C92" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="D90" s="93" t="s">
+      <c r="D92" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="E90" s="93" t="s">
+      <c r="E92" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="F90" s="104"/>
-      <c r="G90" s="104"/>
-      <c r="H90" s="104"/>
-      <c r="I90" s="106"/>
-      <c r="J90" s="93"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="17"/>
-      <c r="M90" s="9"/>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91" s="94"/>
-      <c r="B91" s="94"/>
-      <c r="C91" s="93"/>
-      <c r="D91" s="93"/>
-      <c r="E91" s="93"/>
-      <c r="F91" s="105"/>
-      <c r="G91" s="105"/>
-      <c r="H91" s="105"/>
-      <c r="I91" s="106"/>
-      <c r="J91" s="93"/>
-      <c r="K91" s="18"/>
-      <c r="L91" s="29"/>
-      <c r="M91" s="15"/>
-    </row>
-    <row r="92" spans="1:13">
-      <c r="A92" s="19">
-        <v>1</v>
-      </c>
-      <c r="B92" s="71"/>
-      <c r="C92" s="78"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="87"/>
-      <c r="G92" s="89"/>
-      <c r="H92" s="89"/>
-      <c r="I92" s="87"/>
-      <c r="J92" s="21"/>
-      <c r="K92" s="21"/>
-      <c r="L92" s="28"/>
-      <c r="M92" s="15"/>
+      <c r="F92" s="101"/>
+      <c r="G92" s="101"/>
+      <c r="H92" s="101"/>
+      <c r="I92" s="103"/>
+      <c r="J92" s="104"/>
+      <c r="K92" s="16"/>
+      <c r="L92" s="17"/>
+      <c r="M92" s="9"/>
     </row>
     <row r="93" spans="1:13">
-      <c r="A93" s="19">
-        <f>A92+1</f>
-        <v>2</v>
-      </c>
-      <c r="B93" s="71"/>
-      <c r="C93" s="78"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="87"/>
-      <c r="G93" s="89"/>
-      <c r="H93" s="89"/>
-      <c r="I93" s="87"/>
-      <c r="J93" s="21"/>
-      <c r="K93" s="21"/>
-      <c r="L93" s="28"/>
+      <c r="A93" s="107"/>
+      <c r="B93" s="107"/>
+      <c r="C93" s="104"/>
+      <c r="D93" s="104"/>
+      <c r="E93" s="104"/>
+      <c r="F93" s="102"/>
+      <c r="G93" s="102"/>
+      <c r="H93" s="102"/>
+      <c r="I93" s="103"/>
+      <c r="J93" s="104"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="29"/>
       <c r="M93" s="15"/>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="19">
-        <f t="shared" ref="A94:A98" si="1">A93+1</f>
-        <v>3</v>
-      </c>
-      <c r="B94" s="72"/>
-      <c r="C94" s="79"/>
+        <v>1</v>
+      </c>
+      <c r="B94" s="71"/>
+      <c r="C94" s="78"/>
       <c r="D94" s="20"/>
       <c r="E94" s="20"/>
       <c r="F94" s="87"/>
@@ -3793,16 +3840,16 @@
       <c r="I94" s="87"/>
       <c r="J94" s="21"/>
       <c r="K94" s="21"/>
-      <c r="L94" s="22"/>
+      <c r="L94" s="28"/>
       <c r="M94" s="15"/>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B95" s="73"/>
-      <c r="C95" s="80"/>
+        <f>A94+1</f>
+        <v>2</v>
+      </c>
+      <c r="B95" s="71"/>
+      <c r="C95" s="78"/>
       <c r="D95" s="20"/>
       <c r="E95" s="20"/>
       <c r="F95" s="87"/>
@@ -3811,16 +3858,16 @@
       <c r="I95" s="87"/>
       <c r="J95" s="21"/>
       <c r="K95" s="21"/>
-      <c r="L95" s="22"/>
+      <c r="L95" s="28"/>
       <c r="M95" s="15"/>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="19">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B96" s="73"/>
-      <c r="C96" s="80"/>
+        <f t="shared" ref="A96:A100" si="1">A95+1</f>
+        <v>3</v>
+      </c>
+      <c r="B96" s="72"/>
+      <c r="C96" s="79"/>
       <c r="D96" s="20"/>
       <c r="E96" s="20"/>
       <c r="F96" s="87"/>
@@ -3835,25 +3882,25 @@
     <row r="97" spans="1:13">
       <c r="A97" s="19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B97" s="73"/>
       <c r="C97" s="80"/>
-      <c r="D97" s="74"/>
-      <c r="E97" s="74"/>
-      <c r="F97" s="88"/>
-      <c r="G97" s="90"/>
-      <c r="H97" s="90"/>
-      <c r="I97" s="88"/>
-      <c r="J97" s="76"/>
-      <c r="K97" s="76"/>
-      <c r="L97" s="77"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="87"/>
+      <c r="G97" s="89"/>
+      <c r="H97" s="89"/>
+      <c r="I97" s="87"/>
+      <c r="J97" s="21"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="22"/>
       <c r="M97" s="15"/>
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="19">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B98" s="73"/>
       <c r="C98" s="80"/>
@@ -3868,54 +3915,91 @@
       <c r="L98" s="22"/>
       <c r="M98" s="15"/>
     </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B99" s="73"/>
+      <c r="C99" s="80"/>
+      <c r="D99" s="74"/>
+      <c r="E99" s="74"/>
+      <c r="F99" s="88"/>
+      <c r="G99" s="90"/>
+      <c r="H99" s="90"/>
+      <c r="I99" s="88"/>
+      <c r="J99" s="76"/>
+      <c r="K99" s="76"/>
+      <c r="L99" s="77"/>
+      <c r="M99" s="15"/>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" s="19">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B100" s="73"/>
+      <c r="C100" s="80"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="20"/>
+      <c r="F100" s="87"/>
+      <c r="G100" s="89"/>
+      <c r="H100" s="89"/>
+      <c r="I100" s="87"/>
+      <c r="J100" s="21"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="22"/>
+      <c r="M100" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="H90:H91"/>
-    <mergeCell ref="I90:J91"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="G90:G91"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
+  <mergeCells count="27">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I63:J64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I61:J62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="H92:H93"/>
+    <mergeCell ref="I92:J93"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="G92:G93"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E102:H102" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E104:H104" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C26" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C27" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F63:G80 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65:G82 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C49:C51" xr:uid="{7DF12094-1903-BC49-BDF2-8CDB3E7A15D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51:C53" xr:uid="{7DF12094-1903-BC49-BDF2-8CDB3E7A15D0}">
       <formula1>httpMethod</formula1>
     </dataValidation>
   </dataValidations>
@@ -3980,7 +4064,7 @@
         <v>31</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" s="56" t="s">
         <v>10</v>
@@ -3999,7 +4083,7 @@
       <c r="D4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="107"/>
+      <c r="F4" s="91"/>
       <c r="H4" s="58"/>
       <c r="J4" s="58"/>
       <c r="L4" s="58"/>
@@ -4009,8 +4093,8 @@
         <v>28</v>
       </c>
       <c r="D5" s="60"/>
-      <c r="F5" s="108" t="s">
-        <v>97</v>
+      <c r="F5" s="92" t="s">
+        <v>96</v>
       </c>
       <c r="H5" s="60" t="s">
         <v>13</v>
@@ -4024,18 +4108,18 @@
     </row>
     <row r="6" spans="1:12">
       <c r="B6" s="61"/>
-      <c r="F6" s="108" t="s">
+      <c r="F6" s="92" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="F7" s="93" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="F7" s="109" t="s">
+    <row r="8" spans="1:12">
+      <c r="F8" s="94" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="F8" s="110" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement issuer parameter to authStore#status and pageTransitData#dataStatus. * correct missing parameters.
</commit_message>
<xml_diff>
--- a/meta/samples/pages/LoginSample.xlsx
+++ b/meta/samples/pages/LoginSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/samples/pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21E667B-2908-014C-962D-31133DBEE23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41264E39-50FD-CB4E-9E68-6363276DBAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -846,14 +846,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>/login</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>login</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>ログイン画面の画面コンポーネントのサンプルです。</t>
     <rPh sb="4" eb="6">
       <t xml:space="preserve">ガメｎ </t>
@@ -949,6 +941,14 @@
     <rPh sb="80" eb="82">
       <t xml:space="preserve">テイギ </t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/loginSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>loginSample</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1829,53 +1829,53 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2290,8 +2290,8 @@
   </sheetPr>
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2406,12 +2406,12 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="113"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="10" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
@@ -2423,12 +2423,12 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="113"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="10" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
@@ -2440,10 +2440,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="112" t="s">
+      <c r="A12" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="113"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2457,10 +2457,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="113"/>
+      <c r="B13" s="112"/>
       <c r="C13" s="86" t="s">
         <v>48</v>
       </c>
@@ -2478,11 +2478,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="114" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="115"/>
-      <c r="E14" s="116"/>
+      <c r="C14" s="113" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="114"/>
+      <c r="E14" s="115"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2623,10 +2623,10 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="104" t="s">
+      <c r="A23" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="105"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="64"/>
       <c r="D23" t="s">
         <v>58</v>
@@ -2638,15 +2638,15 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="104" t="s">
+      <c r="A24" s="116" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="117"/>
+      <c r="C24" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
         <v>105</v>
-      </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" t="s">
-        <v>107</v>
       </c>
       <c r="E24"/>
       <c r="F24"/>
@@ -2670,10 +2670,10 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="104" t="s">
+      <c r="A26" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="105"/>
+      <c r="B26" s="117"/>
       <c r="C26" s="64" t="s">
         <v>14</v>
       </c>
@@ -2687,10 +2687,10 @@
       <c r="I26"/>
     </row>
     <row r="27" spans="1:13" s="32" customFormat="1">
-      <c r="A27" s="104" t="s">
+      <c r="A27" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="105"/>
+      <c r="B27" s="117"/>
       <c r="C27" s="64" t="s">
         <v>14</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
@@ -2776,7 +2776,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C32" s="101"/>
       <c r="D32" s="101"/>
@@ -2998,7 +2998,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="38"/>
@@ -3081,7 +3081,7 @@
         <v>63</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D50" s="42" t="s">
         <v>64</v>
@@ -3104,10 +3104,10 @@
         <v>87</v>
       </c>
       <c r="C51" s="95" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D51" s="98" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E51" s="39"/>
       <c r="F51" s="68"/>
@@ -3293,49 +3293,49 @@
       <c r="M62" s="15"/>
     </row>
     <row r="63" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A63" s="107" t="s">
+      <c r="A63" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="107" t="s">
+      <c r="B63" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="106" t="s">
+      <c r="C63" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="106" t="s">
+      <c r="D63" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="106" t="s">
+      <c r="E63" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="110" t="s">
+      <c r="F63" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="G63" s="110" t="s">
+      <c r="G63" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="H63" s="108" t="s">
+      <c r="H63" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="I63" s="106" t="s">
+      <c r="I63" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="J63" s="106"/>
+      <c r="J63" s="107"/>
       <c r="K63" s="16"/>
       <c r="L63" s="17"/>
       <c r="M63" s="9"/>
     </row>
     <row r="64" spans="1:13">
-      <c r="A64" s="107"/>
-      <c r="B64" s="107"/>
-      <c r="C64" s="106"/>
-      <c r="D64" s="106"/>
-      <c r="E64" s="106"/>
-      <c r="F64" s="111"/>
-      <c r="G64" s="111"/>
-      <c r="H64" s="109"/>
-      <c r="I64" s="106"/>
-      <c r="J64" s="106"/>
+      <c r="A64" s="110"/>
+      <c r="B64" s="110"/>
+      <c r="C64" s="107"/>
+      <c r="D64" s="107"/>
+      <c r="E64" s="107"/>
+      <c r="F64" s="109"/>
+      <c r="G64" s="109"/>
+      <c r="H64" s="119"/>
+      <c r="I64" s="107"/>
+      <c r="J64" s="107"/>
       <c r="K64" s="18"/>
       <c r="L64" s="29"/>
       <c r="M64" s="15"/>
@@ -3787,41 +3787,41 @@
       <c r="M91" s="15"/>
     </row>
     <row r="92" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A92" s="107" t="s">
+      <c r="A92" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B92" s="107" t="s">
+      <c r="B92" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="C92" s="106" t="s">
+      <c r="C92" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="D92" s="106" t="s">
+      <c r="D92" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="E92" s="106" t="s">
+      <c r="E92" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="F92" s="117"/>
-      <c r="G92" s="117"/>
-      <c r="H92" s="117"/>
-      <c r="I92" s="119"/>
-      <c r="J92" s="106"/>
+      <c r="F92" s="104"/>
+      <c r="G92" s="104"/>
+      <c r="H92" s="104"/>
+      <c r="I92" s="106"/>
+      <c r="J92" s="107"/>
       <c r="K92" s="16"/>
       <c r="L92" s="17"/>
       <c r="M92" s="9"/>
     </row>
     <row r="93" spans="1:13">
-      <c r="A93" s="107"/>
-      <c r="B93" s="107"/>
-      <c r="C93" s="106"/>
-      <c r="D93" s="106"/>
-      <c r="E93" s="106"/>
-      <c r="F93" s="118"/>
-      <c r="G93" s="118"/>
-      <c r="H93" s="118"/>
-      <c r="I93" s="119"/>
-      <c r="J93" s="106"/>
+      <c r="A93" s="110"/>
+      <c r="B93" s="110"/>
+      <c r="C93" s="107"/>
+      <c r="D93" s="107"/>
+      <c r="E93" s="107"/>
+      <c r="F93" s="105"/>
+      <c r="G93" s="105"/>
+      <c r="H93" s="105"/>
+      <c r="I93" s="106"/>
+      <c r="J93" s="107"/>
       <c r="K93" s="18"/>
       <c r="L93" s="29"/>
       <c r="M93" s="15"/>
@@ -3953,21 +3953,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="H92:H93"/>
-    <mergeCell ref="I92:J93"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="G92:G93"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="I63:J64"/>
@@ -3980,6 +3965,21 @@
     <mergeCell ref="F63:F64"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="H92:H93"/>
+    <mergeCell ref="I92:J93"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="G92:G93"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
@@ -4064,7 +4064,7 @@
         <v>31</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H3" s="56" t="s">
         <v>10</v>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="D5" s="60"/>
       <c r="F5" s="92" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H5" s="60" t="s">
         <v>13</v>
@@ -4109,17 +4109,17 @@
     <row r="6" spans="1:12">
       <c r="B6" s="61"/>
       <c r="F6" s="92" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="F7" s="93" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="F8" s="94" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get response infromation from http headers.
</commit_message>
<xml_diff>
--- a/meta/samples/pages/LoginSample.xlsx
+++ b/meta/samples/pages/LoginSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/samples/pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41264E39-50FD-CB4E-9E68-6363276DBAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFB17AE-DDA1-8A42-A978-F00973EF95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="111">
   <si>
     <t>パッケージ</t>
   </si>
@@ -949,6 +949,21 @@
   </si>
   <si>
     <t>loginSample</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>SampleMethodTest</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>dapanda-api-coreに定義されているAPIです。</t>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { SampleMethodTestPostRequest } from "%/samples/api/SampleMethodTestPostRequest"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1646,27 +1661,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1675,38 +1689,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1718,8 +1725,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1752,18 +1759,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1773,12 +1778,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1792,16 +1797,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1820,36 +1825,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1865,17 +1870,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2288,10 +2290,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2333,9 +2335,6 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
@@ -2347,12 +2346,9 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="35"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
@@ -2364,12 +2360,9 @@
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="35"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
@@ -2381,12 +2374,9 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -2396,99 +2386,81 @@
       <c r="C9" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="111" t="s">
+      <c r="A10" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="112"/>
+      <c r="B10" s="100"/>
       <c r="C10" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="112"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="111" t="s">
+      <c r="A12" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="112"/>
+      <c r="B12" s="100"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="33"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="112"/>
-      <c r="C13" s="86" t="s">
+      <c r="B13" s="100"/>
+      <c r="C13" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
     </row>
     <row r="14" spans="1:11" ht="45" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="113" t="s">
+      <c r="C14" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="114"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
@@ -2500,19 +2472,13 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-    </row>
-    <row r="16" spans="1:11" s="32" customFormat="1">
-      <c r="A16" s="62" t="s">
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="55" t="s">
         <v>27</v>
       </c>
       <c r="D16" t="s">
@@ -2520,46 +2486,46 @@
       </c>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:13" s="32" customFormat="1">
-      <c r="A17" s="62" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="55"/>
       <c r="D17" t="s">
         <v>36</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:13" s="32" customFormat="1">
-      <c r="A18" s="62" t="s">
+    <row r="18" spans="1:12">
+      <c r="A18" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="55"/>
       <c r="D18" t="s">
         <v>36</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
+      <c r="G18"/>
+      <c r="H18"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:13" s="32" customFormat="1">
-      <c r="A19" s="62" t="s">
+    <row r="19" spans="1:12">
+      <c r="A19" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D19" t="s">
@@ -2567,16 +2533,16 @@
       </c>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
+      <c r="G19"/>
+      <c r="H19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:13" s="32" customFormat="1">
-      <c r="A20" s="62" t="s">
+    <row r="20" spans="1:12">
+      <c r="A20" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="64" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
@@ -2584,16 +2550,16 @@
       </c>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
+      <c r="G20"/>
+      <c r="H20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:13" s="32" customFormat="1">
-      <c r="A21" s="62" t="s">
+    <row r="21" spans="1:12">
+      <c r="A21" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="s">
@@ -2601,16 +2567,16 @@
       </c>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:13" s="32" customFormat="1">
-      <c r="A22" s="62" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D22" t="s">
@@ -2618,31 +2584,31 @@
       </c>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
+      <c r="G22"/>
+      <c r="H22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="116" t="s">
+    <row r="23" spans="1:12">
+      <c r="A23" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="117"/>
-      <c r="C23" s="64"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="55"/>
       <c r="D23" t="s">
         <v>58</v>
       </c>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="116" t="s">
+    <row r="24" spans="1:12">
+      <c r="A24" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="117"/>
-      <c r="C24" s="64" t="s">
+      <c r="B24" s="92"/>
+      <c r="C24" s="55" t="s">
         <v>104</v>
       </c>
       <c r="D24" t="s">
@@ -2654,27 +2620,27 @@
       <c r="H24"/>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="62" t="s">
+    <row r="25" spans="1:12">
+      <c r="A25" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="64" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
+      <c r="G25"/>
+      <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="116" t="s">
+    <row r="26" spans="1:12">
+      <c r="A26" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="117"/>
-      <c r="C26" s="64" t="s">
+      <c r="B26" s="92"/>
+      <c r="C26" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
@@ -2682,1308 +2648,1227 @@
       </c>
       <c r="E26"/>
       <c r="F26"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
+      <c r="G26"/>
+      <c r="H26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:13" s="32" customFormat="1">
-      <c r="A27" s="116" t="s">
+    <row r="27" spans="1:12">
+      <c r="A27" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="92"/>
+      <c r="C27" s="55" t="s">
         <v>14</v>
       </c>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
+      <c r="G27"/>
+      <c r="H27"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="1:13" s="37" customFormat="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="30" t="s">
+    <row r="28" spans="1:12">
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="44" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="47" t="s">
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="51">
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="43">
         <v>1</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" spans="1:13" s="32" customFormat="1">
-      <c r="A32" s="51">
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="43">
         <v>2</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="101"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="103"/>
-      <c r="H32" s="103"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
       <c r="J32"/>
       <c r="K32"/>
       <c r="L32"/>
     </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="51"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="35"/>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="52"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="35"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="30" t="s">
+    <row r="33" spans="1:12">
+      <c r="A33" s="43"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="44"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="44" t="s">
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="47" t="s">
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="67"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="35"/>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="51">
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="43">
         <v>1</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="35"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="51">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="43">
         <v>2</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="35"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="52">
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="44">
         <v>3</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="35"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="83"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="83"/>
-      <c r="B42" s="67"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="30" t="s">
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="73"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="73"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="44" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="43"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="47" t="s">
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="67"/>
-      <c r="G44" s="67"/>
-      <c r="H44" s="67"/>
-      <c r="I44" s="67"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="35"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="51">
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="43">
         <v>1</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="68"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="35"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" s="51"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="68"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="68"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="35"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="52"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="68"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="43">
+        <v>1</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="43"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="44"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="30" t="s">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="44" t="s">
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="47" t="s">
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B51" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="47" t="s">
+      <c r="C51" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="42" t="s">
+      <c r="D51" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="82"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="44"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="45"/>
-      <c r="M50" s="35"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="51">
+      <c r="E51" s="72"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="43">
         <v>1</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B52" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="95" t="s">
+      <c r="C52" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="D51" s="98" t="s">
+      <c r="D52" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="36"/>
-      <c r="L51" s="36"/>
-      <c r="M51" s="35"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="51"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="96"/>
-      <c r="D52" s="99"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="36"/>
-      <c r="L52" s="36"/>
-      <c r="M52" s="35"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="52"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="97"/>
-      <c r="D53" s="100"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="36"/>
-      <c r="L53" s="36"/>
-      <c r="M53" s="35"/>
+      <c r="A53" s="43">
+        <v>2</v>
+      </c>
+      <c r="B53" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="E53" s="35"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="83"/>
-      <c r="B54" s="84"/>
-      <c r="C54" s="85"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="36"/>
-      <c r="L54" s="36"/>
-      <c r="M54" s="35"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="87"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="73"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="44" t="s">
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43"/>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="47" t="s">
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B57" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="42"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="82"/>
-      <c r="F56" s="67" t="s">
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="72"/>
+      <c r="F57" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="G56" s="67"/>
-      <c r="H56" s="67"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="45"/>
-      <c r="M56" s="35"/>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57" s="51"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="68"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="36"/>
-      <c r="K57" s="36"/>
-      <c r="L57" s="36"/>
-      <c r="M57" s="35"/>
+      <c r="G57" s="57"/>
+      <c r="H57" s="57"/>
+      <c r="I57" s="57"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="51"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="68"/>
-      <c r="H58" s="68"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="36"/>
-      <c r="K58" s="36"/>
-      <c r="L58" s="36"/>
-      <c r="M58" s="35"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="52"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="68"/>
-      <c r="G59" s="68"/>
-      <c r="H59" s="68"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="36"/>
-      <c r="K59" s="36"/>
-      <c r="L59" s="36"/>
-      <c r="M59" s="35"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="58"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="58"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13" t="s">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62"/>
+      <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="3" t="s">
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="6"/>
-      <c r="M62" s="15"/>
-    </row>
-    <row r="63" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A63" s="110" t="s">
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A64" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="110" t="s">
+      <c r="B64" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="107" t="s">
+      <c r="C64" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="107" t="s">
+      <c r="D64" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="107" t="s">
+      <c r="E64" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="108" t="s">
+      <c r="F64" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="G63" s="108" t="s">
+      <c r="G64" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="H63" s="118" t="s">
+      <c r="H64" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="I63" s="107" t="s">
+      <c r="I64" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="J63" s="107"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="9"/>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64" s="110"/>
-      <c r="B64" s="110"/>
-      <c r="C64" s="107"/>
-      <c r="D64" s="107"/>
-      <c r="E64" s="107"/>
-      <c r="F64" s="109"/>
-      <c r="G64" s="109"/>
-      <c r="H64" s="119"/>
-      <c r="I64" s="107"/>
-      <c r="J64" s="107"/>
-      <c r="K64" s="18"/>
-      <c r="L64" s="29"/>
-      <c r="M64" s="15"/>
+      <c r="J64" s="93"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="16"/>
+      <c r="M64" s="9"/>
     </row>
     <row r="65" spans="1:13">
-      <c r="A65" s="19">
+      <c r="A65" s="94"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="93"/>
+      <c r="D65" s="93"/>
+      <c r="E65" s="93"/>
+      <c r="F65" s="98"/>
+      <c r="G65" s="98"/>
+      <c r="H65" s="96"/>
+      <c r="I65" s="93"/>
+      <c r="J65" s="93"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="14"/>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="18">
         <v>1</v>
       </c>
-      <c r="B65" s="71"/>
-      <c r="C65" s="78"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="69"/>
-      <c r="H65" s="69"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="21"/>
-      <c r="K65" s="21"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="15"/>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66" s="19">
-        <f>A65+1</f>
+      <c r="B66" s="61"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="59"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="27"/>
+      <c r="M66" s="14"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="18">
+        <f>A66+1</f>
         <v>2</v>
       </c>
-      <c r="B66" s="71"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="69"/>
-      <c r="H66" s="69"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="15"/>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67" s="19">
-        <f t="shared" ref="A67:A81" si="0">A66+1</f>
+      <c r="B67" s="61"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="59"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="27"/>
+      <c r="M67" s="14"/>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="18">
+        <f t="shared" ref="A68:A82" si="0">A67+1</f>
         <v>3</v>
       </c>
-      <c r="B67" s="72"/>
-      <c r="C67" s="79"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="15"/>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68" s="19">
+      <c r="B68" s="62"/>
+      <c r="C68" s="69"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="14"/>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B68" s="73"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="69"/>
-      <c r="H68" s="69"/>
-      <c r="I68" s="20"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21"/>
-      <c r="L68" s="22"/>
-      <c r="M68" s="15"/>
-    </row>
-    <row r="69" spans="1:13">
-      <c r="A69" s="19">
+      <c r="B69" s="63"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="14"/>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B69" s="73"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="69"/>
-      <c r="H69" s="69"/>
-      <c r="I69" s="20"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="15"/>
-    </row>
-    <row r="70" spans="1:13">
-      <c r="A70" s="19">
+      <c r="B70" s="63"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="14"/>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B70" s="73"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="76"/>
-      <c r="K70" s="76"/>
-      <c r="L70" s="77"/>
-      <c r="M70" s="15"/>
-    </row>
-    <row r="71" spans="1:13">
-      <c r="A71" s="19">
+      <c r="B71" s="63"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="65"/>
+      <c r="H71" s="65"/>
+      <c r="I71" s="64"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="66"/>
+      <c r="L71" s="67"/>
+      <c r="M71" s="14"/>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B71" s="73"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="69"/>
-      <c r="H71" s="69"/>
-      <c r="I71" s="20"/>
-      <c r="J71" s="21"/>
-      <c r="K71" s="21"/>
-      <c r="L71" s="22"/>
-      <c r="M71" s="15"/>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="A72" s="19">
+      <c r="B72" s="63"/>
+      <c r="C72" s="70"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="21"/>
+      <c r="M72" s="14"/>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B72" s="73"/>
-      <c r="C72" s="80"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="74"/>
-      <c r="J72" s="76"/>
-      <c r="K72" s="76"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="15"/>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="A73" s="19">
+      <c r="B73" s="63"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="65"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="64"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+      <c r="L73" s="67"/>
+      <c r="M73" s="14"/>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B73" s="73"/>
-      <c r="C73" s="80"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="74"/>
-      <c r="J73" s="76"/>
-      <c r="K73" s="76"/>
-      <c r="L73" s="77"/>
-      <c r="M73" s="15"/>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" s="19">
+      <c r="B74" s="63"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="64"/>
+      <c r="J74" s="66"/>
+      <c r="K74" s="66"/>
+      <c r="L74" s="67"/>
+      <c r="M74" s="14"/>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B74" s="73"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="69"/>
-      <c r="H74" s="69"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="21"/>
-      <c r="K74" s="21"/>
-      <c r="L74" s="22"/>
-      <c r="M74" s="15"/>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" s="19">
+      <c r="B75" s="63"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="59"/>
+      <c r="H75" s="59"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="20"/>
+      <c r="K75" s="20"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="14"/>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B75" s="73"/>
-      <c r="C75" s="80"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="74"/>
-      <c r="J75" s="76"/>
-      <c r="K75" s="76"/>
-      <c r="L75" s="77"/>
-      <c r="M75" s="15"/>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76" s="19">
+      <c r="B76" s="63"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="64"/>
+      <c r="J76" s="66"/>
+      <c r="K76" s="66"/>
+      <c r="L76" s="67"/>
+      <c r="M76" s="14"/>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B76" s="73"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
-      <c r="I76" s="74"/>
-      <c r="J76" s="76"/>
-      <c r="K76" s="76"/>
-      <c r="L76" s="77"/>
-      <c r="M76" s="15"/>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="19">
+      <c r="B77" s="63"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="66"/>
+      <c r="K77" s="66"/>
+      <c r="L77" s="67"/>
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="A78" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B77" s="73"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="69"/>
-      <c r="H77" s="69"/>
-      <c r="I77" s="20"/>
-      <c r="J77" s="21"/>
-      <c r="K77" s="21"/>
-      <c r="L77" s="22"/>
-      <c r="M77" s="15"/>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="A78" s="19">
+      <c r="B78" s="63"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="20"/>
+      <c r="K78" s="20"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="14"/>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B78" s="73"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="75"/>
-      <c r="I78" s="74"/>
-      <c r="J78" s="76"/>
-      <c r="K78" s="76"/>
-      <c r="L78" s="77"/>
-      <c r="M78" s="15"/>
-    </row>
-    <row r="79" spans="1:13">
-      <c r="A79" s="19">
+      <c r="B79" s="63"/>
+      <c r="C79" s="70"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
+      <c r="F79" s="64"/>
+      <c r="G79" s="65"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="66"/>
+      <c r="K79" s="66"/>
+      <c r="L79" s="67"/>
+      <c r="M79" s="14"/>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B79" s="73"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-      <c r="F79" s="74"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
-      <c r="I79" s="74"/>
-      <c r="J79" s="76"/>
-      <c r="K79" s="76"/>
-      <c r="L79" s="77"/>
-      <c r="M79" s="15"/>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80" s="19">
+      <c r="B80" s="63"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="66"/>
+      <c r="K80" s="66"/>
+      <c r="L80" s="67"/>
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B80" s="73"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="69"/>
-      <c r="H80" s="69"/>
-      <c r="I80" s="20"/>
-      <c r="J80" s="21"/>
-      <c r="K80" s="21"/>
-      <c r="L80" s="22"/>
-      <c r="M80" s="15"/>
-    </row>
-    <row r="81" spans="1:13">
-      <c r="A81" s="19">
+      <c r="B81" s="63"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="59"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="20"/>
+      <c r="L81" s="21"/>
+      <c r="M81" s="14"/>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B81" s="73"/>
-      <c r="C81" s="80"/>
-      <c r="D81" s="74"/>
-      <c r="E81" s="74"/>
-      <c r="F81" s="74"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="I81" s="74"/>
-      <c r="J81" s="76"/>
-      <c r="K81" s="76"/>
-      <c r="L81" s="77"/>
-      <c r="M81" s="15"/>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="70"/>
-      <c r="H82" s="70"/>
-      <c r="I82" s="25"/>
-      <c r="J82" s="26"/>
-      <c r="K82" s="26"/>
-      <c r="L82" s="27"/>
-      <c r="M82" s="15"/>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="30" t="s">
+      <c r="B82" s="63"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
+      <c r="F82" s="64"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="64"/>
+      <c r="J82" s="66"/>
+      <c r="K82" s="66"/>
+      <c r="L82" s="67"/>
+      <c r="M82" s="14"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="22"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="60"/>
+      <c r="H83" s="60"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="25"/>
+      <c r="K83" s="25"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="14"/>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="31"/>
-      <c r="C84" s="31"/>
-      <c r="D84" s="31"/>
-      <c r="E84" s="81"/>
-      <c r="F84" s="44" t="s">
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="71"/>
+      <c r="F85" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G84" s="44"/>
-      <c r="H84" s="44"/>
-      <c r="I84" s="44"/>
-      <c r="J84" s="43"/>
-      <c r="K84" s="43"/>
-      <c r="L84" s="43"/>
-      <c r="M84" s="43"/>
-    </row>
-    <row r="85" spans="1:13">
-      <c r="A85" s="47" t="s">
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="42" t="s">
+      <c r="B86" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="82"/>
-      <c r="F85" s="67"/>
-      <c r="G85" s="67"/>
-      <c r="H85" s="67"/>
-      <c r="I85" s="67"/>
-      <c r="J85" s="44"/>
-      <c r="K85" s="45"/>
-      <c r="L85" s="45"/>
-      <c r="M85" s="35"/>
-    </row>
-    <row r="86" spans="1:13">
-      <c r="A86" s="51"/>
-      <c r="B86" s="46"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="39"/>
-      <c r="F86" s="68"/>
-      <c r="G86" s="68"/>
-      <c r="H86" s="68"/>
-      <c r="I86" s="34"/>
-      <c r="J86" s="36"/>
-      <c r="K86" s="36"/>
-      <c r="L86" s="36"/>
-      <c r="M86" s="35"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="72"/>
+      <c r="F86" s="57"/>
+      <c r="G86" s="57"/>
+      <c r="H86" s="57"/>
+      <c r="I86" s="57"/>
+      <c r="K86" s="37"/>
+      <c r="L86" s="37"/>
     </row>
     <row r="87" spans="1:13">
-      <c r="A87" s="51"/>
-      <c r="B87" s="46"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="41"/>
-      <c r="F87" s="68"/>
-      <c r="G87" s="68"/>
-      <c r="H87" s="68"/>
-      <c r="I87" s="34"/>
-      <c r="J87" s="36"/>
-      <c r="K87" s="36"/>
-      <c r="L87" s="36"/>
-      <c r="M87" s="35"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="58"/>
+      <c r="H87" s="58"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
     </row>
     <row r="88" spans="1:13">
-      <c r="A88" s="52"/>
-      <c r="B88" s="48"/>
-      <c r="C88" s="49"/>
-      <c r="D88" s="49"/>
-      <c r="E88" s="50"/>
-      <c r="F88" s="68"/>
-      <c r="G88" s="68"/>
-      <c r="H88" s="68"/>
-      <c r="I88" s="34"/>
-      <c r="J88" s="36"/>
-      <c r="K88" s="36"/>
-      <c r="L88" s="36"/>
-      <c r="M88" s="35"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="34"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="35"/>
+      <c r="F88" s="58"/>
+      <c r="G88" s="58"/>
+      <c r="H88" s="58"/>
+      <c r="J88"/>
+      <c r="K88"/>
+      <c r="L88"/>
     </row>
     <row r="89" spans="1:13">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
+      <c r="A89" s="44"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="41"/>
+      <c r="D89" s="41"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="58"/>
+      <c r="G89" s="58"/>
+      <c r="H89" s="58"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
     </row>
     <row r="90" spans="1:13">
-      <c r="A90" s="13"/>
-      <c r="B90" s="13" t="s">
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91"/>
+      <c r="B91" t="s">
         <v>68</v>
       </c>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91" s="3" t="s">
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+      <c r="J91"/>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="14"/>
-      <c r="K91" s="14"/>
-      <c r="L91" s="6"/>
-      <c r="M91" s="15"/>
-    </row>
-    <row r="92" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A92" s="110" t="s">
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="13"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="14"/>
+    </row>
+    <row r="93" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A93" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B92" s="110" t="s">
+      <c r="B93" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="C92" s="107" t="s">
+      <c r="C93" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="D92" s="107" t="s">
+      <c r="D93" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="E92" s="107" t="s">
+      <c r="E93" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="F92" s="104"/>
-      <c r="G92" s="104"/>
-      <c r="H92" s="104"/>
-      <c r="I92" s="106"/>
-      <c r="J92" s="107"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="17"/>
-      <c r="M92" s="9"/>
-    </row>
-    <row r="93" spans="1:13">
-      <c r="A93" s="110"/>
-      <c r="B93" s="110"/>
-      <c r="C93" s="107"/>
-      <c r="D93" s="107"/>
-      <c r="E93" s="107"/>
-      <c r="F93" s="105"/>
-      <c r="G93" s="105"/>
-      <c r="H93" s="105"/>
+      <c r="F93" s="104"/>
+      <c r="G93" s="104"/>
+      <c r="H93" s="104"/>
       <c r="I93" s="106"/>
-      <c r="J93" s="107"/>
-      <c r="K93" s="18"/>
-      <c r="L93" s="29"/>
-      <c r="M93" s="15"/>
+      <c r="J93" s="93"/>
+      <c r="K93" s="15"/>
+      <c r="L93" s="16"/>
+      <c r="M93" s="9"/>
     </row>
     <row r="94" spans="1:13">
-      <c r="A94" s="19">
+      <c r="A94" s="94"/>
+      <c r="B94" s="94"/>
+      <c r="C94" s="93"/>
+      <c r="D94" s="93"/>
+      <c r="E94" s="93"/>
+      <c r="F94" s="105"/>
+      <c r="G94" s="105"/>
+      <c r="H94" s="105"/>
+      <c r="I94" s="106"/>
+      <c r="J94" s="93"/>
+      <c r="K94" s="17"/>
+      <c r="L94" s="28"/>
+      <c r="M94" s="14"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="18">
         <v>1</v>
       </c>
-      <c r="B94" s="71"/>
-      <c r="C94" s="78"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="87"/>
-      <c r="G94" s="89"/>
-      <c r="H94" s="89"/>
-      <c r="I94" s="87"/>
-      <c r="J94" s="21"/>
-      <c r="K94" s="21"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="15"/>
-    </row>
-    <row r="95" spans="1:13">
-      <c r="A95" s="19">
-        <f>A94+1</f>
+      <c r="B95" s="61"/>
+      <c r="C95" s="68"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="77"/>
+      <c r="G95" s="79"/>
+      <c r="H95" s="79"/>
+      <c r="I95" s="77"/>
+      <c r="J95" s="20"/>
+      <c r="K95" s="20"/>
+      <c r="L95" s="27"/>
+      <c r="M95" s="14"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="18">
+        <f>A95+1</f>
         <v>2</v>
       </c>
-      <c r="B95" s="71"/>
-      <c r="C95" s="78"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="87"/>
-      <c r="G95" s="89"/>
-      <c r="H95" s="89"/>
-      <c r="I95" s="87"/>
-      <c r="J95" s="21"/>
-      <c r="K95" s="21"/>
-      <c r="L95" s="28"/>
-      <c r="M95" s="15"/>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96" s="19">
-        <f t="shared" ref="A96:A100" si="1">A95+1</f>
+      <c r="B96" s="61"/>
+      <c r="C96" s="68"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="77"/>
+      <c r="G96" s="79"/>
+      <c r="H96" s="79"/>
+      <c r="I96" s="77"/>
+      <c r="J96" s="20"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="27"/>
+      <c r="M96" s="14"/>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="18">
+        <f t="shared" ref="A97:A101" si="1">A96+1</f>
         <v>3</v>
       </c>
-      <c r="B96" s="72"/>
-      <c r="C96" s="79"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="87"/>
-      <c r="G96" s="89"/>
-      <c r="H96" s="89"/>
-      <c r="I96" s="87"/>
-      <c r="J96" s="21"/>
-      <c r="K96" s="21"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="15"/>
-    </row>
-    <row r="97" spans="1:13">
-      <c r="A97" s="19">
+      <c r="B97" s="62"/>
+      <c r="C97" s="69"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="77"/>
+      <c r="G97" s="79"/>
+      <c r="H97" s="79"/>
+      <c r="I97" s="77"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="21"/>
+      <c r="M97" s="14"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="18">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B97" s="73"/>
-      <c r="C97" s="80"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="87"/>
-      <c r="G97" s="89"/>
-      <c r="H97" s="89"/>
-      <c r="I97" s="87"/>
-      <c r="J97" s="21"/>
-      <c r="K97" s="21"/>
-      <c r="L97" s="22"/>
-      <c r="M97" s="15"/>
-    </row>
-    <row r="98" spans="1:13">
-      <c r="A98" s="19">
+      <c r="B98" s="63"/>
+      <c r="C98" s="70"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="77"/>
+      <c r="G98" s="79"/>
+      <c r="H98" s="79"/>
+      <c r="I98" s="77"/>
+      <c r="J98" s="20"/>
+      <c r="K98" s="20"/>
+      <c r="L98" s="21"/>
+      <c r="M98" s="14"/>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="18">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B98" s="73"/>
-      <c r="C98" s="80"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="87"/>
-      <c r="G98" s="89"/>
-      <c r="H98" s="89"/>
-      <c r="I98" s="87"/>
-      <c r="J98" s="21"/>
-      <c r="K98" s="21"/>
-      <c r="L98" s="22"/>
-      <c r="M98" s="15"/>
-    </row>
-    <row r="99" spans="1:13">
-      <c r="A99" s="19">
+      <c r="B99" s="63"/>
+      <c r="C99" s="70"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="77"/>
+      <c r="G99" s="79"/>
+      <c r="H99" s="79"/>
+      <c r="I99" s="77"/>
+      <c r="J99" s="20"/>
+      <c r="K99" s="20"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="14"/>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" s="18">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B99" s="73"/>
-      <c r="C99" s="80"/>
-      <c r="D99" s="74"/>
-      <c r="E99" s="74"/>
-      <c r="F99" s="88"/>
-      <c r="G99" s="90"/>
-      <c r="H99" s="90"/>
-      <c r="I99" s="88"/>
-      <c r="J99" s="76"/>
-      <c r="K99" s="76"/>
-      <c r="L99" s="77"/>
-      <c r="M99" s="15"/>
-    </row>
-    <row r="100" spans="1:13">
-      <c r="A100" s="19">
+      <c r="B100" s="63"/>
+      <c r="C100" s="70"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="78"/>
+      <c r="G100" s="80"/>
+      <c r="H100" s="80"/>
+      <c r="I100" s="78"/>
+      <c r="J100" s="66"/>
+      <c r="K100" s="66"/>
+      <c r="L100" s="67"/>
+      <c r="M100" s="14"/>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B100" s="73"/>
-      <c r="C100" s="80"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="87"/>
-      <c r="G100" s="89"/>
-      <c r="H100" s="89"/>
-      <c r="I100" s="87"/>
-      <c r="J100" s="21"/>
-      <c r="K100" s="21"/>
-      <c r="L100" s="22"/>
-      <c r="M100" s="15"/>
+      <c r="B101" s="63"/>
+      <c r="C101" s="70"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="77"/>
+      <c r="G101" s="79"/>
+      <c r="H101" s="79"/>
+      <c r="I101" s="77"/>
+      <c r="J101" s="20"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I63:J64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="F93:F94"/>
+    <mergeCell ref="H93:H94"/>
+    <mergeCell ref="I93:J94"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="G93:G94"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="E93:E94"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="H92:H93"/>
-    <mergeCell ref="I92:J93"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="G92:G93"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I64:J65"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E104:H104" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E105:H105" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3993,13 +3878,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65:G82 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F66:G83 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51:C53" xr:uid="{7DF12094-1903-BC49-BDF2-8CDB3E7A15D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C52:C54" xr:uid="{7DF12094-1903-BC49-BDF2-8CDB3E7A15D0}">
       <formula1>httpMethod</formula1>
     </dataValidation>
   </dataValidations>
@@ -4024,101 +3909,101 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="55" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="55" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="55" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="55" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="55" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="55" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="55" bestFit="1" customWidth="1"/>
-    <col min="13" max="253" width="8.83203125" style="55" customWidth="1"/>
-    <col min="254" max="16384" width="10.83203125" style="55"/>
+    <col min="1" max="3" width="8.83203125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="47" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="47" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="47" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="13" max="253" width="8.83203125" style="47" customWidth="1"/>
+    <col min="254" max="16384" width="10.83203125" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="19">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="54" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="46" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="48" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="H4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="L4" s="58"/>
+      <c r="F4" s="81"/>
+      <c r="H4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="L4" s="50"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="F5" s="92" t="s">
+      <c r="D5" s="52"/>
+      <c r="F5" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="60" t="s">
+      <c r="L5" s="52" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="B6" s="61"/>
-      <c r="F6" s="92" t="s">
+      <c r="B6" s="53"/>
+      <c r="F6" s="82" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="F7" s="93" t="s">
+      <c r="F7" s="83" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="F8" s="94" t="s">
+      <c r="F8" s="84" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.0.7: Adapt Path and Query on Post/Put. * even need empty object {} if no body.
</commit_message>
<xml_diff>
--- a/meta/samples/pages/LoginSample.xlsx
+++ b/meta/samples/pages/LoginSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/samples/pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFB17AE-DDA1-8A42-A978-F00973EF95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9EEEB1-E672-9F41-8587-04A007FF54B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
   <si>
     <t>パッケージ</t>
   </si>
@@ -964,6 +964,20 @@
   </si>
   <si>
     <t>import { SampleMethodTestPostRequest } from "%/samples/api/SampleMethodTestPostRequest"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { SampleMethodTestPutRequest } from "%/samples/api/SampleMethodTestPutRequest"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>import { SampleMethodTestGetRequest } from "%/samples/api/SampleMethodTestGetRequest"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -2290,10 +2304,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2925,7 +2939,8 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="43">
-        <v>1</v>
+        <f>A45+1</f>
+        <v>2</v>
       </c>
       <c r="B46" s="38" t="s">
         <v>110</v>
@@ -2941,11 +2956,16 @@
       <c r="L46"/>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="43"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="35"/>
+      <c r="A47" s="43">
+        <f>A46+1</f>
+        <v>3</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="33"/>
       <c r="F47" s="58"/>
       <c r="G47" s="58"/>
       <c r="H47" s="58"/>
@@ -2954,11 +2974,16 @@
       <c r="L47"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="44"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
+      <c r="A48" s="43">
+        <f>A47+1</f>
+        <v>4</v>
+      </c>
+      <c r="B48" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="33"/>
       <c r="F48" s="58"/>
       <c r="G48" s="58"/>
       <c r="H48" s="58"/>
@@ -2966,99 +2991,91 @@
       <c r="K48"/>
       <c r="L48"/>
     </row>
-    <row r="49" spans="1:13">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="H49"/>
-      <c r="I49"/>
+    <row r="49" spans="1:12">
+      <c r="A49" s="43"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
       <c r="J49"/>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="29" t="s">
+      <c r="K49"/>
+      <c r="L49"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="44"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="71"/>
-      <c r="F50" s="1" t="s">
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="39" t="s">
+    <row r="53" spans="1:12">
+      <c r="A53" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="B53" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C53" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D53" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="E51" s="72"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="43">
+      <c r="E53" s="72"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="43">
         <v>1</v>
       </c>
-      <c r="B52" s="38" t="s">
+      <c r="B54" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="85" t="s">
+      <c r="C54" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="88" t="s">
+      <c r="D54" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="E52" s="33"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="43">
-        <v>2</v>
-      </c>
-      <c r="B53" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="D53" s="89" t="s">
-        <v>109</v>
-      </c>
-      <c r="E53" s="35"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="J53"/>
-      <c r="K53"/>
-      <c r="L53"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="44"/>
-      <c r="B54" s="40"/>
-      <c r="C54" s="87"/>
-      <c r="D54" s="90"/>
-      <c r="E54" s="42"/>
+      <c r="E54" s="33"/>
       <c r="F54" s="58"/>
       <c r="G54" s="58"/>
       <c r="H54" s="58"/>
@@ -3066,12 +3083,20 @@
       <c r="K54"/>
       <c r="L54"/>
     </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="73"/>
-      <c r="B55" s="74"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
+    <row r="55" spans="1:12">
+      <c r="A55" s="43">
+        <v>2</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="35"/>
       <c r="F55" s="58"/>
       <c r="G55" s="58"/>
       <c r="H55" s="58"/>
@@ -3079,43 +3104,54 @@
       <c r="K55"/>
       <c r="L55"/>
     </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="71"/>
-      <c r="F56" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="G57" s="57"/>
-      <c r="H57" s="57"/>
-      <c r="I57" s="57"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="37"/>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="43"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="33"/>
+    <row r="56" spans="1:12">
+      <c r="A56" s="43">
+        <v>3</v>
+      </c>
+      <c r="B56" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="35"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="43">
+        <v>3</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="86" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="89" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" s="35"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="44"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="87"/>
+      <c r="D58" s="90"/>
+      <c r="E58" s="42"/>
       <c r="F58" s="58"/>
       <c r="G58" s="58"/>
       <c r="H58" s="58"/>
@@ -3123,12 +3159,12 @@
       <c r="K58"/>
       <c r="L58"/>
     </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="43"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="35"/>
+    <row r="59" spans="1:12">
+      <c r="A59" s="73"/>
+      <c r="B59" s="74"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="75"/>
       <c r="F59" s="58"/>
       <c r="G59" s="58"/>
       <c r="H59" s="58"/>
@@ -3136,188 +3172,173 @@
       <c r="K59"/>
       <c r="L59"/>
     </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="44"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="J60"/>
-      <c r="K60"/>
-      <c r="L60"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="J61"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62"/>
-      <c r="B62" t="s">
+    <row r="60" spans="1:12">
+      <c r="A60" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="57"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="43"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="58"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="43"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="58"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="58"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="44"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="41"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="58"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="58"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65"/>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66"/>
+      <c r="B66" t="s">
         <v>61</v>
       </c>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
-      <c r="J62"/>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" s="3" t="s">
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="6"/>
-      <c r="M63" s="14"/>
-    </row>
-    <row r="64" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A64" s="94" t="s">
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="14"/>
+    </row>
+    <row r="68" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A68" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="94" t="s">
+      <c r="B68" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="93" t="s">
+      <c r="C68" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="93" t="s">
+      <c r="D68" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="93" t="s">
+      <c r="E68" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="97" t="s">
+      <c r="F68" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="G64" s="97" t="s">
+      <c r="G68" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="H64" s="95" t="s">
+      <c r="H68" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="I64" s="93" t="s">
+      <c r="I68" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="J64" s="93"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="16"/>
-      <c r="M64" s="9"/>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65" s="94"/>
-      <c r="B65" s="94"/>
-      <c r="C65" s="93"/>
-      <c r="D65" s="93"/>
-      <c r="E65" s="93"/>
-      <c r="F65" s="98"/>
-      <c r="G65" s="98"/>
-      <c r="H65" s="96"/>
-      <c r="I65" s="93"/>
-      <c r="J65" s="93"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="14"/>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66" s="18">
-        <v>1</v>
-      </c>
-      <c r="B66" s="61"/>
-      <c r="C66" s="68"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="59"/>
-      <c r="H66" s="59"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="20"/>
-      <c r="K66" s="20"/>
-      <c r="L66" s="27"/>
-      <c r="M66" s="14"/>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67" s="18">
-        <f>A66+1</f>
-        <v>2</v>
-      </c>
-      <c r="B67" s="61"/>
-      <c r="C67" s="68"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="59"/>
-      <c r="H67" s="59"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="20"/>
-      <c r="K67" s="20"/>
-      <c r="L67" s="27"/>
-      <c r="M67" s="14"/>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68" s="18">
-        <f t="shared" ref="A68:A82" si="0">A67+1</f>
-        <v>3</v>
-      </c>
-      <c r="B68" s="62"/>
-      <c r="C68" s="69"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="59"/>
-      <c r="H68" s="59"/>
-      <c r="I68" s="19"/>
-      <c r="J68" s="20"/>
-      <c r="K68" s="20"/>
-      <c r="L68" s="21"/>
-      <c r="M68" s="14"/>
+      <c r="J68" s="93"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="16"/>
+      <c r="M68" s="9"/>
     </row>
     <row r="69" spans="1:13">
-      <c r="A69" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B69" s="63"/>
-      <c r="C69" s="70"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="59"/>
-      <c r="H69" s="59"/>
-      <c r="I69" s="19"/>
-      <c r="J69" s="20"/>
-      <c r="K69" s="20"/>
-      <c r="L69" s="21"/>
+      <c r="A69" s="94"/>
+      <c r="B69" s="94"/>
+      <c r="C69" s="93"/>
+      <c r="D69" s="93"/>
+      <c r="E69" s="93"/>
+      <c r="F69" s="98"/>
+      <c r="G69" s="98"/>
+      <c r="H69" s="96"/>
+      <c r="I69" s="93"/>
+      <c r="J69" s="93"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="28"/>
       <c r="M69" s="14"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="18">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B70" s="63"/>
-      <c r="C70" s="70"/>
+        <v>1</v>
+      </c>
+      <c r="B70" s="61"/>
+      <c r="C70" s="68"/>
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
       <c r="F70" s="19"/>
@@ -3326,34 +3347,34 @@
       <c r="I70" s="19"/>
       <c r="J70" s="20"/>
       <c r="K70" s="20"/>
-      <c r="L70" s="21"/>
+      <c r="L70" s="27"/>
       <c r="M70" s="14"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B71" s="63"/>
-      <c r="C71" s="70"/>
-      <c r="D71" s="64"/>
-      <c r="E71" s="64"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="65"/>
-      <c r="H71" s="65"/>
-      <c r="I71" s="64"/>
-      <c r="J71" s="66"/>
-      <c r="K71" s="66"/>
-      <c r="L71" s="67"/>
+        <f>A70+1</f>
+        <v>2</v>
+      </c>
+      <c r="B71" s="61"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="20"/>
+      <c r="K71" s="20"/>
+      <c r="L71" s="27"/>
       <c r="M71" s="14"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="18">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B72" s="63"/>
-      <c r="C72" s="70"/>
+        <f t="shared" ref="A72:A86" si="0">A71+1</f>
+        <v>3</v>
+      </c>
+      <c r="B72" s="62"/>
+      <c r="C72" s="69"/>
       <c r="D72" s="19"/>
       <c r="E72" s="19"/>
       <c r="F72" s="19"/>
@@ -3368,79 +3389,79 @@
     <row r="73" spans="1:13">
       <c r="A73" s="18">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B73" s="63"/>
       <c r="C73" s="70"/>
-      <c r="D73" s="64"/>
-      <c r="E73" s="64"/>
-      <c r="F73" s="64"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="65"/>
-      <c r="I73" s="64"/>
-      <c r="J73" s="66"/>
-      <c r="K73" s="66"/>
-      <c r="L73" s="67"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="L73" s="21"/>
       <c r="M73" s="14"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="18">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B74" s="63"/>
       <c r="C74" s="70"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="64"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="65"/>
-      <c r="I74" s="64"/>
-      <c r="J74" s="66"/>
-      <c r="K74" s="66"/>
-      <c r="L74" s="67"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="20"/>
+      <c r="L74" s="21"/>
       <c r="M74" s="14"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="18">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B75" s="63"/>
       <c r="C75" s="70"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="59"/>
-      <c r="H75" s="59"/>
-      <c r="I75" s="19"/>
-      <c r="J75" s="20"/>
-      <c r="K75" s="20"/>
-      <c r="L75" s="21"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="65"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="64"/>
+      <c r="J75" s="66"/>
+      <c r="K75" s="66"/>
+      <c r="L75" s="67"/>
       <c r="M75" s="14"/>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="18">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B76" s="63"/>
       <c r="C76" s="70"/>
-      <c r="D76" s="64"/>
-      <c r="E76" s="64"/>
-      <c r="F76" s="64"/>
-      <c r="G76" s="65"/>
-      <c r="H76" s="65"/>
-      <c r="I76" s="64"/>
-      <c r="J76" s="66"/>
-      <c r="K76" s="66"/>
-      <c r="L76" s="67"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="21"/>
       <c r="M76" s="14"/>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="18">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B77" s="63"/>
       <c r="C77" s="70"/>
@@ -3458,43 +3479,43 @@
     <row r="78" spans="1:13">
       <c r="A78" s="18">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B78" s="63"/>
       <c r="C78" s="70"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="59"/>
-      <c r="H78" s="59"/>
-      <c r="I78" s="19"/>
-      <c r="J78" s="20"/>
-      <c r="K78" s="20"/>
-      <c r="L78" s="21"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="64"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="66"/>
+      <c r="L78" s="67"/>
       <c r="M78" s="14"/>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B79" s="63"/>
       <c r="C79" s="70"/>
-      <c r="D79" s="64"/>
-      <c r="E79" s="64"/>
-      <c r="F79" s="64"/>
-      <c r="G79" s="65"/>
-      <c r="H79" s="65"/>
-      <c r="I79" s="64"/>
-      <c r="J79" s="66"/>
-      <c r="K79" s="66"/>
-      <c r="L79" s="67"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="59"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="20"/>
+      <c r="K79" s="20"/>
+      <c r="L79" s="21"/>
       <c r="M79" s="14"/>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B80" s="63"/>
       <c r="C80" s="70"/>
@@ -3512,283 +3533,283 @@
     <row r="81" spans="1:13">
       <c r="A81" s="18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B81" s="63"/>
       <c r="C81" s="70"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="59"/>
-      <c r="H81" s="59"/>
-      <c r="I81" s="19"/>
-      <c r="J81" s="20"/>
-      <c r="K81" s="20"/>
-      <c r="L81" s="21"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="65"/>
+      <c r="H81" s="65"/>
+      <c r="I81" s="64"/>
+      <c r="J81" s="66"/>
+      <c r="K81" s="66"/>
+      <c r="L81" s="67"/>
       <c r="M81" s="14"/>
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="18">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B82" s="63"/>
       <c r="C82" s="70"/>
-      <c r="D82" s="64"/>
-      <c r="E82" s="64"/>
-      <c r="F82" s="64"/>
-      <c r="G82" s="65"/>
-      <c r="H82" s="65"/>
-      <c r="I82" s="64"/>
-      <c r="J82" s="66"/>
-      <c r="K82" s="66"/>
-      <c r="L82" s="67"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="59"/>
+      <c r="H82" s="59"/>
+      <c r="I82" s="19"/>
+      <c r="J82" s="20"/>
+      <c r="K82" s="20"/>
+      <c r="L82" s="21"/>
       <c r="M82" s="14"/>
     </row>
     <row r="83" spans="1:13">
-      <c r="A83" s="22"/>
-      <c r="B83" s="23"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="60"/>
-      <c r="H83" s="60"/>
-      <c r="I83" s="24"/>
-      <c r="J83" s="25"/>
-      <c r="K83" s="25"/>
-      <c r="L83" s="26"/>
+      <c r="A83" s="18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B83" s="63"/>
+      <c r="C83" s="70"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="65"/>
+      <c r="H83" s="65"/>
+      <c r="I83" s="64"/>
+      <c r="J83" s="66"/>
+      <c r="K83" s="66"/>
+      <c r="L83" s="67"/>
       <c r="M83" s="14"/>
     </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B84" s="63"/>
+      <c r="C84" s="70"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
+      <c r="F84" s="64"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+      <c r="I84" s="64"/>
+      <c r="J84" s="66"/>
+      <c r="K84" s="66"/>
+      <c r="L84" s="67"/>
+      <c r="M84" s="14"/>
+    </row>
     <row r="85" spans="1:13">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B85" s="63"/>
+      <c r="C85" s="70"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="59"/>
+      <c r="H85" s="59"/>
+      <c r="I85" s="19"/>
+      <c r="J85" s="20"/>
+      <c r="K85" s="20"/>
+      <c r="L85" s="21"/>
+      <c r="M85" s="14"/>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B86" s="63"/>
+      <c r="C86" s="70"/>
+      <c r="D86" s="64"/>
+      <c r="E86" s="64"/>
+      <c r="F86" s="64"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="64"/>
+      <c r="J86" s="66"/>
+      <c r="K86" s="66"/>
+      <c r="L86" s="67"/>
+      <c r="M86" s="14"/>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="22"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="60"/>
+      <c r="H87" s="60"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="25"/>
+      <c r="K87" s="25"/>
+      <c r="L87" s="26"/>
+      <c r="M87" s="14"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B85" s="30"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="71"/>
-      <c r="F85" s="1" t="s">
+      <c r="B89" s="30"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="71"/>
+      <c r="F89" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
-      <c r="A86" s="39" t="s">
+    <row r="90" spans="1:13">
+      <c r="A90" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="36" t="s">
+      <c r="B90" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="72"/>
-      <c r="F86" s="57"/>
-      <c r="G86" s="57"/>
-      <c r="H86" s="57"/>
-      <c r="I86" s="57"/>
-      <c r="K86" s="37"/>
-      <c r="L86" s="37"/>
-    </row>
-    <row r="87" spans="1:13">
-      <c r="A87" s="43"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
-      <c r="E87" s="33"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="58"/>
-      <c r="H87" s="58"/>
-      <c r="J87"/>
-      <c r="K87"/>
-      <c r="L87"/>
-    </row>
-    <row r="88" spans="1:13">
-      <c r="A88" s="43"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="34"/>
-      <c r="D88" s="34"/>
-      <c r="E88" s="35"/>
-      <c r="F88" s="58"/>
-      <c r="G88" s="58"/>
-      <c r="H88" s="58"/>
-      <c r="J88"/>
-      <c r="K88"/>
-      <c r="L88"/>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89" s="44"/>
-      <c r="B89" s="40"/>
-      <c r="C89" s="41"/>
-      <c r="D89" s="41"/>
-      <c r="E89" s="42"/>
-      <c r="F89" s="58"/>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
-      <c r="J89"/>
-      <c r="K89"/>
-      <c r="L89"/>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="D90"/>
-      <c r="E90"/>
-      <c r="F90"/>
-      <c r="G90"/>
-      <c r="H90"/>
-      <c r="I90"/>
-      <c r="J90"/>
+      <c r="C90" s="36"/>
+      <c r="D90" s="36"/>
+      <c r="E90" s="72"/>
+      <c r="F90" s="57"/>
+      <c r="G90" s="57"/>
+      <c r="H90" s="57"/>
+      <c r="I90" s="57"/>
+      <c r="K90" s="37"/>
+      <c r="L90" s="37"/>
     </row>
     <row r="91" spans="1:13">
-      <c r="A91"/>
-      <c r="B91" t="s">
+      <c r="A91" s="43"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="33"/>
+      <c r="F91" s="58"/>
+      <c r="G91" s="58"/>
+      <c r="H91" s="58"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="43"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="34"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="35"/>
+      <c r="F92" s="58"/>
+      <c r="G92" s="58"/>
+      <c r="H92" s="58"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92"/>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="44"/>
+      <c r="B93" s="40"/>
+      <c r="C93" s="41"/>
+      <c r="D93" s="41"/>
+      <c r="E93" s="42"/>
+      <c r="F93" s="58"/>
+      <c r="G93" s="58"/>
+      <c r="H93" s="58"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95"/>
+      <c r="B95" t="s">
         <v>68</v>
       </c>
-      <c r="C91"/>
-      <c r="D91"/>
-      <c r="E91"/>
-      <c r="F91"/>
-      <c r="G91"/>
-      <c r="H91"/>
-      <c r="I91"/>
-      <c r="J91"/>
-    </row>
-    <row r="92" spans="1:13">
-      <c r="A92" s="3" t="s">
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="6"/>
-      <c r="M92" s="14"/>
-    </row>
-    <row r="93" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A93" s="94" t="s">
+      <c r="B96" s="13"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="14"/>
+    </row>
+    <row r="97" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A97" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B93" s="94" t="s">
+      <c r="B97" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="C93" s="93" t="s">
+      <c r="C97" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="D93" s="93" t="s">
+      <c r="D97" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="E93" s="93" t="s">
+      <c r="E97" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="F93" s="104"/>
-      <c r="G93" s="104"/>
-      <c r="H93" s="104"/>
-      <c r="I93" s="106"/>
-      <c r="J93" s="93"/>
-      <c r="K93" s="15"/>
-      <c r="L93" s="16"/>
-      <c r="M93" s="9"/>
-    </row>
-    <row r="94" spans="1:13">
-      <c r="A94" s="94"/>
-      <c r="B94" s="94"/>
-      <c r="C94" s="93"/>
-      <c r="D94" s="93"/>
-      <c r="E94" s="93"/>
-      <c r="F94" s="105"/>
-      <c r="G94" s="105"/>
-      <c r="H94" s="105"/>
-      <c r="I94" s="106"/>
-      <c r="J94" s="93"/>
-      <c r="K94" s="17"/>
-      <c r="L94" s="28"/>
-      <c r="M94" s="14"/>
-    </row>
-    <row r="95" spans="1:13">
-      <c r="A95" s="18">
-        <v>1</v>
-      </c>
-      <c r="B95" s="61"/>
-      <c r="C95" s="68"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="77"/>
-      <c r="G95" s="79"/>
-      <c r="H95" s="79"/>
-      <c r="I95" s="77"/>
-      <c r="J95" s="20"/>
-      <c r="K95" s="20"/>
-      <c r="L95" s="27"/>
-      <c r="M95" s="14"/>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96" s="18">
-        <f>A95+1</f>
-        <v>2</v>
-      </c>
-      <c r="B96" s="61"/>
-      <c r="C96" s="68"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="77"/>
-      <c r="G96" s="79"/>
-      <c r="H96" s="79"/>
-      <c r="I96" s="77"/>
-      <c r="J96" s="20"/>
-      <c r="K96" s="20"/>
-      <c r="L96" s="27"/>
-      <c r="M96" s="14"/>
-    </row>
-    <row r="97" spans="1:13">
-      <c r="A97" s="18">
-        <f t="shared" ref="A97:A101" si="1">A96+1</f>
-        <v>3</v>
-      </c>
-      <c r="B97" s="62"/>
-      <c r="C97" s="69"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="77"/>
-      <c r="G97" s="79"/>
-      <c r="H97" s="79"/>
-      <c r="I97" s="77"/>
-      <c r="J97" s="20"/>
-      <c r="K97" s="20"/>
-      <c r="L97" s="21"/>
-      <c r="M97" s="14"/>
+      <c r="F97" s="104"/>
+      <c r="G97" s="104"/>
+      <c r="H97" s="104"/>
+      <c r="I97" s="106"/>
+      <c r="J97" s="93"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="16"/>
+      <c r="M97" s="9"/>
     </row>
     <row r="98" spans="1:13">
-      <c r="A98" s="18">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B98" s="63"/>
-      <c r="C98" s="70"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="77"/>
-      <c r="G98" s="79"/>
-      <c r="H98" s="79"/>
-      <c r="I98" s="77"/>
-      <c r="J98" s="20"/>
-      <c r="K98" s="20"/>
-      <c r="L98" s="21"/>
+      <c r="A98" s="94"/>
+      <c r="B98" s="94"/>
+      <c r="C98" s="93"/>
+      <c r="D98" s="93"/>
+      <c r="E98" s="93"/>
+      <c r="F98" s="105"/>
+      <c r="G98" s="105"/>
+      <c r="H98" s="105"/>
+      <c r="I98" s="106"/>
+      <c r="J98" s="93"/>
+      <c r="K98" s="17"/>
+      <c r="L98" s="28"/>
       <c r="M98" s="14"/>
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="18">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B99" s="63"/>
-      <c r="C99" s="70"/>
+        <v>1</v>
+      </c>
+      <c r="B99" s="61"/>
+      <c r="C99" s="68"/>
       <c r="D99" s="19"/>
       <c r="E99" s="19"/>
       <c r="F99" s="77"/>
@@ -3797,34 +3818,34 @@
       <c r="I99" s="77"/>
       <c r="J99" s="20"/>
       <c r="K99" s="20"/>
-      <c r="L99" s="21"/>
+      <c r="L99" s="27"/>
       <c r="M99" s="14"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="18">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B100" s="63"/>
-      <c r="C100" s="70"/>
-      <c r="D100" s="64"/>
-      <c r="E100" s="64"/>
-      <c r="F100" s="78"/>
-      <c r="G100" s="80"/>
-      <c r="H100" s="80"/>
-      <c r="I100" s="78"/>
-      <c r="J100" s="66"/>
-      <c r="K100" s="66"/>
-      <c r="L100" s="67"/>
+        <f>A99+1</f>
+        <v>2</v>
+      </c>
+      <c r="B100" s="61"/>
+      <c r="C100" s="68"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="77"/>
+      <c r="G100" s="79"/>
+      <c r="H100" s="79"/>
+      <c r="I100" s="77"/>
+      <c r="J100" s="20"/>
+      <c r="K100" s="20"/>
+      <c r="L100" s="27"/>
       <c r="M100" s="14"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="18">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B101" s="63"/>
-      <c r="C101" s="70"/>
+        <f t="shared" ref="A101:A105" si="1">A100+1</f>
+        <v>3</v>
+      </c>
+      <c r="B101" s="62"/>
+      <c r="C101" s="69"/>
       <c r="D101" s="19"/>
       <c r="E101" s="19"/>
       <c r="F101" s="77"/>
@@ -3836,18 +3857,90 @@
       <c r="L101" s="21"/>
       <c r="M101" s="14"/>
     </row>
+    <row r="102" spans="1:13">
+      <c r="A102" s="18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B102" s="63"/>
+      <c r="C102" s="70"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="77"/>
+      <c r="G102" s="79"/>
+      <c r="H102" s="79"/>
+      <c r="I102" s="77"/>
+      <c r="J102" s="20"/>
+      <c r="K102" s="20"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="14"/>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103" s="18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B103" s="63"/>
+      <c r="C103" s="70"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="77"/>
+      <c r="G103" s="79"/>
+      <c r="H103" s="79"/>
+      <c r="I103" s="77"/>
+      <c r="J103" s="20"/>
+      <c r="K103" s="20"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="14"/>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="A104" s="18">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B104" s="63"/>
+      <c r="C104" s="70"/>
+      <c r="D104" s="64"/>
+      <c r="E104" s="64"/>
+      <c r="F104" s="78"/>
+      <c r="G104" s="80"/>
+      <c r="H104" s="80"/>
+      <c r="I104" s="78"/>
+      <c r="J104" s="66"/>
+      <c r="K104" s="66"/>
+      <c r="L104" s="67"/>
+      <c r="M104" s="14"/>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="A105" s="18">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B105" s="63"/>
+      <c r="C105" s="70"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="77"/>
+      <c r="G105" s="79"/>
+      <c r="H105" s="79"/>
+      <c r="I105" s="77"/>
+      <c r="J105" s="20"/>
+      <c r="K105" s="20"/>
+      <c r="L105" s="21"/>
+      <c r="M105" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F93:F94"/>
-    <mergeCell ref="H93:H94"/>
-    <mergeCell ref="I93:J94"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="G93:G94"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="H97:H98"/>
+    <mergeCell ref="I97:J98"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="G97:G98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="E97:E98"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -3855,20 +3948,20 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I64:J65"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="I68:J69"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="F68:F69"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A24:B24"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E105:H105" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E109:H109" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3878,13 +3971,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F66:G83 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F70:G87 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C52:C54" xr:uid="{7DF12094-1903-BC49-BDF2-8CDB3E7A15D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54:C58" xr:uid="{7DF12094-1903-BC49-BDF2-8CDB3E7A15D0}">
       <formula1>httpMethod</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>